<commit_message>
Changes in CFRP UP
</commit_message>
<xml_diff>
--- a/Data/Antera_inputs.xlsx
+++ b/Data/Antera_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://embraer-my.sharepoint.com/personal/giacomo_parolin_embraer_com_br/Documents/2_LCE/1_DfE/PEE 28/Antera/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="258" documentId="13_ncr:1_{7DBD5BA2-9E9A-472F-BFB5-8083F6B4D3CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{53991E46-7856-4BF5-8FBF-42DC63977E1B}"/>
+  <xr:revisionPtr revIDLastSave="285" documentId="13_ncr:1_{7DBD5BA2-9E9A-472F-BFB5-8083F6B4D3CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{01449176-B1B9-417D-8963-8B56C7E2492C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="285">
   <si>
     <t>nominal</t>
   </si>
@@ -996,6 +996,24 @@
   </si>
   <si>
     <t>takt-time in days in Brazil</t>
+  </si>
+  <si>
+    <t>p_ldf_CFRP</t>
+  </si>
+  <si>
+    <t>p_incin_CFRP</t>
+  </si>
+  <si>
+    <t>p_recycl_CFRP</t>
+  </si>
+  <si>
+    <t>percentage of landfilled CFRP</t>
+  </si>
+  <si>
+    <t>percentage of incinerated CFRP</t>
+  </si>
+  <si>
+    <t>percentage of recycled CFRP</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1024,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1057,12 +1075,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1257,7 +1269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1345,67 +1357,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1454,14 +1406,80 @@
     <xf numFmtId="1" fontId="6" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1798,8 +1816,8 @@
   <dimension ref="A1:L122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19:A21"/>
+      <pane ySplit="3" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1814,14 +1832,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="67" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" s="29"/>
@@ -1852,7 +1870,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="65" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -1878,7 +1896,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="41"/>
+      <c r="A5" s="65"/>
       <c r="B5" s="8" t="s">
         <v>276</v>
       </c>
@@ -1902,7 +1920,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="41"/>
+      <c r="A6" s="65"/>
       <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
@@ -1923,7 +1941,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="41"/>
+      <c r="A7" s="65"/>
       <c r="B7" s="8" t="s">
         <v>205</v>
       </c>
@@ -1945,7 +1963,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="41"/>
+      <c r="A8" s="65"/>
       <c r="B8" s="8" t="s">
         <v>206</v>
       </c>
@@ -1968,7 +1986,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="41"/>
+      <c r="A9" s="65"/>
       <c r="B9" s="8" t="s">
         <v>207</v>
       </c>
@@ -1989,7 +2007,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="41"/>
+      <c r="A10" s="65"/>
       <c r="B10" s="8" t="s">
         <v>55</v>
       </c>
@@ -2012,7 +2030,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="41"/>
+      <c r="A11" s="65"/>
       <c r="B11" s="8" t="s">
         <v>214</v>
       </c>
@@ -2033,7 +2051,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="41"/>
+      <c r="A12" s="65"/>
       <c r="B12" s="8" t="s">
         <v>123</v>
       </c>
@@ -2054,7 +2072,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="41"/>
+      <c r="A13" s="65"/>
       <c r="B13" s="8" t="s">
         <v>208</v>
       </c>
@@ -2075,7 +2093,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="41"/>
+      <c r="A14" s="65"/>
       <c r="B14" s="8" t="s">
         <v>209</v>
       </c>
@@ -2096,7 +2114,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="41"/>
+      <c r="A15" s="65"/>
       <c r="B15" s="8" t="s">
         <v>210</v>
       </c>
@@ -2117,7 +2135,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="41"/>
+      <c r="A16" s="65"/>
       <c r="B16" s="8" t="s">
         <v>211</v>
       </c>
@@ -2138,7 +2156,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="41"/>
+      <c r="A17" s="65"/>
       <c r="B17" s="8" t="s">
         <v>212</v>
       </c>
@@ -2159,7 +2177,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="78"/>
+      <c r="A18" s="66"/>
       <c r="B18" s="8" t="s">
         <v>213</v>
       </c>
@@ -2180,105 +2198,105 @@
       </c>
     </row>
     <row r="19" spans="1:7" s="31" customFormat="1" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="79" t="s">
+      <c r="A19" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="74" t="s">
+      <c r="B19" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="75">
+      <c r="C19" s="55">
         <f>107087/500*C23</f>
         <v>107087</v>
       </c>
-      <c r="D19" s="75">
+      <c r="D19" s="55">
         <f>107087/500*D23</f>
         <v>85669.6</v>
       </c>
-      <c r="E19" s="75">
+      <c r="E19" s="55">
         <f>107087/500*E23</f>
         <v>128504.40000000001</v>
       </c>
-      <c r="F19" s="76" t="s">
+      <c r="F19" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="G19" s="76" t="s">
+      <c r="G19" s="56" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="80"/>
-      <c r="B20" s="74" t="s">
+      <c r="A20" s="70"/>
+      <c r="B20" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="75">
+      <c r="C20" s="55">
         <f>190/500*C23</f>
         <v>190</v>
       </c>
-      <c r="D20" s="75">
+      <c r="D20" s="55">
         <f t="shared" ref="D20:E20" si="4">190/500*D23</f>
         <v>152</v>
       </c>
-      <c r="E20" s="75">
+      <c r="E20" s="55">
         <f t="shared" si="4"/>
         <v>228</v>
       </c>
-      <c r="F20" s="76" t="s">
+      <c r="F20" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="G20" s="76" t="s">
+      <c r="G20" s="56" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="80"/>
-      <c r="B21" s="74" t="s">
+      <c r="A21" s="70"/>
+      <c r="B21" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="75">
+      <c r="C21" s="55">
         <f>3000/4/500*C23</f>
         <v>750</v>
       </c>
-      <c r="D21" s="75">
+      <c r="D21" s="55">
         <f t="shared" ref="D21:E21" si="5">3000/4/500*D23</f>
         <v>600</v>
       </c>
-      <c r="E21" s="75">
+      <c r="E21" s="55">
         <f t="shared" si="5"/>
         <v>900</v>
       </c>
-      <c r="F21" s="76" t="s">
+      <c r="F21" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="G21" s="76" t="s">
+      <c r="G21" s="56" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="51" t="s">
+      <c r="A22" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="59" t="s">
+      <c r="B22" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="77">
+      <c r="C22" s="57">
         <v>48</v>
       </c>
-      <c r="D22" s="77">
+      <c r="D22" s="57">
         <v>48</v>
       </c>
-      <c r="E22" s="77">
+      <c r="E22" s="57">
         <f>C22*1.2</f>
         <v>57.599999999999994</v>
       </c>
-      <c r="F22" s="61" t="s">
+      <c r="F22" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="G22" s="61" t="s">
+      <c r="G22" s="41" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="52"/>
+      <c r="A23" s="72"/>
       <c r="B23" s="22" t="s">
         <v>65</v>
       </c>
@@ -2301,7 +2319,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="52"/>
+      <c r="A24" s="72"/>
       <c r="B24" s="22" t="s">
         <v>263</v>
       </c>
@@ -2325,7 +2343,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="52"/>
+      <c r="A25" s="72"/>
       <c r="B25" s="22" t="s">
         <v>124</v>
       </c>
@@ -2349,53 +2367,53 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="52"/>
-      <c r="B26" s="59" t="s">
+      <c r="A26" s="72"/>
+      <c r="B26" s="39" t="s">
         <v>264</v>
       </c>
-      <c r="C26" s="60">
+      <c r="C26" s="40">
         <v>10</v>
       </c>
-      <c r="D26" s="60">
+      <c r="D26" s="40">
         <f>C26*0.4</f>
         <v>4</v>
       </c>
-      <c r="E26" s="60">
+      <c r="E26" s="40">
         <f>C26*1.6</f>
         <v>16</v>
       </c>
-      <c r="F26" s="61" t="s">
+      <c r="F26" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="G26" s="61" t="s">
+      <c r="G26" s="41" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="52"/>
-      <c r="B27" s="59" t="s">
+      <c r="A27" s="72"/>
+      <c r="B27" s="39" t="s">
         <v>265</v>
       </c>
-      <c r="C27" s="60">
+      <c r="C27" s="40">
         <v>10</v>
       </c>
-      <c r="D27" s="60">
+      <c r="D27" s="40">
         <f>C27*0.4</f>
         <v>4</v>
       </c>
-      <c r="E27" s="60">
+      <c r="E27" s="40">
         <f>C27*1.6</f>
         <v>16</v>
       </c>
-      <c r="F27" s="61" t="s">
+      <c r="F27" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="G27" s="61" t="s">
+      <c r="G27" s="41" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="52"/>
+      <c r="A28" s="72"/>
       <c r="B28" s="22" t="s">
         <v>71</v>
       </c>
@@ -2418,7 +2436,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="52"/>
+      <c r="A29" s="72"/>
       <c r="B29" s="22" t="s">
         <v>72</v>
       </c>
@@ -2441,7 +2459,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="52"/>
+      <c r="A30" s="72"/>
       <c r="B30" s="22" t="s">
         <v>75</v>
       </c>
@@ -2464,7 +2482,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="44" t="s">
+      <c r="A31" s="73" t="s">
         <v>34</v>
       </c>
       <c r="B31" s="9" t="s">
@@ -2487,7 +2505,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="45"/>
+      <c r="A32" s="74"/>
       <c r="B32" s="9" t="s">
         <v>12</v>
       </c>
@@ -2508,7 +2526,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="45"/>
+      <c r="A33" s="74"/>
       <c r="B33" s="9" t="s">
         <v>222</v>
       </c>
@@ -2529,7 +2547,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="45"/>
+      <c r="A34" s="74"/>
       <c r="B34" s="9" t="s">
         <v>19</v>
       </c>
@@ -2550,7 +2568,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="45"/>
+      <c r="A35" s="74"/>
       <c r="B35" s="9" t="s">
         <v>13</v>
       </c>
@@ -2571,7 +2589,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="45"/>
+      <c r="A36" s="74"/>
       <c r="B36" s="9" t="s">
         <v>14</v>
       </c>
@@ -2592,7 +2610,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="45"/>
+      <c r="A37" s="74"/>
       <c r="B37" s="9" t="s">
         <v>15</v>
       </c>
@@ -2613,7 +2631,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="45"/>
+      <c r="A38" s="74"/>
       <c r="B38" s="9" t="s">
         <v>16</v>
       </c>
@@ -2634,7 +2652,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="45"/>
+      <c r="A39" s="74"/>
       <c r="B39" s="9" t="s">
         <v>226</v>
       </c>
@@ -2655,7 +2673,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="45"/>
+      <c r="A40" s="74"/>
       <c r="B40" s="9" t="s">
         <v>20</v>
       </c>
@@ -2676,7 +2694,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="45"/>
+      <c r="A41" s="74"/>
       <c r="B41" s="9" t="s">
         <v>17</v>
       </c>
@@ -2697,7 +2715,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="45"/>
+      <c r="A42" s="74"/>
       <c r="B42" s="9" t="s">
         <v>18</v>
       </c>
@@ -2718,171 +2736,171 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="46" t="s">
+      <c r="A43" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="62" t="s">
+      <c r="B43" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="C43" s="65">
+      <c r="C43" s="45">
         <v>100000</v>
       </c>
-      <c r="D43" s="65">
+      <c r="D43" s="45">
         <f t="shared" si="6"/>
         <v>80000</v>
       </c>
-      <c r="E43" s="65">
+      <c r="E43" s="45">
         <f t="shared" si="7"/>
         <v>120000</v>
       </c>
-      <c r="F43" s="64" t="s">
+      <c r="F43" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="G43" s="66" t="s">
+      <c r="G43" s="46" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="47"/>
-      <c r="B44" s="62" t="s">
+      <c r="A44" s="76"/>
+      <c r="B44" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="C44" s="65">
+      <c r="C44" s="45">
         <v>20000</v>
       </c>
-      <c r="D44" s="65">
+      <c r="D44" s="45">
         <f t="shared" si="6"/>
         <v>16000</v>
       </c>
-      <c r="E44" s="65">
+      <c r="E44" s="45">
         <f t="shared" si="7"/>
         <v>24000</v>
       </c>
-      <c r="F44" s="64" t="s">
+      <c r="F44" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="G44" s="66" t="s">
+      <c r="G44" s="46" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="47"/>
-      <c r="B45" s="62" t="s">
+      <c r="A45" s="76"/>
+      <c r="B45" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="C45" s="65">
+      <c r="C45" s="45">
         <v>40000</v>
       </c>
-      <c r="D45" s="65">
+      <c r="D45" s="45">
         <f t="shared" si="6"/>
         <v>32000</v>
       </c>
-      <c r="E45" s="65">
+      <c r="E45" s="45">
         <f t="shared" si="7"/>
         <v>48000</v>
       </c>
-      <c r="F45" s="64" t="s">
+      <c r="F45" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="G45" s="66" t="s">
+      <c r="G45" s="46" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="47"/>
-      <c r="B46" s="62" t="s">
+      <c r="A46" s="76"/>
+      <c r="B46" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="C46" s="63">
+      <c r="C46" s="43">
         <f>80/18000*(2*C24)</f>
         <v>169.44</v>
       </c>
-      <c r="D46" s="63">
+      <c r="D46" s="43">
         <f t="shared" si="6"/>
         <v>135.55199999999999</v>
       </c>
-      <c r="E46" s="63">
+      <c r="E46" s="43">
         <f t="shared" si="7"/>
         <v>203.328</v>
       </c>
-      <c r="F46" s="64" t="s">
+      <c r="F46" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="G46" s="66" t="s">
+      <c r="G46" s="46" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="47"/>
-      <c r="B47" s="62" t="s">
+      <c r="A47" s="76"/>
+      <c r="B47" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C47" s="63">
+      <c r="C47" s="43">
         <f>64/18000*(2*C24)</f>
         <v>135.55199999999999</v>
       </c>
-      <c r="D47" s="63">
+      <c r="D47" s="43">
         <f t="shared" si="6"/>
         <v>108.44159999999999</v>
       </c>
-      <c r="E47" s="63">
+      <c r="E47" s="43">
         <f t="shared" si="7"/>
         <v>162.66239999999999</v>
       </c>
-      <c r="F47" s="64" t="s">
+      <c r="F47" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="G47" s="66" t="s">
+      <c r="G47" s="46" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="47"/>
-      <c r="B48" s="62" t="s">
+      <c r="A48" s="76"/>
+      <c r="B48" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="C48" s="63">
+      <c r="C48" s="43">
         <f>(15+15+20+20+20+20+19+19+20+20+20+20+20+20)/1000/18000*(2*C24)</f>
         <v>0.56762400000000002</v>
       </c>
-      <c r="D48" s="63">
+      <c r="D48" s="43">
         <f t="shared" si="6"/>
         <v>0.45409920000000004</v>
       </c>
-      <c r="E48" s="63">
+      <c r="E48" s="43">
         <f t="shared" si="7"/>
         <v>0.6811488</v>
       </c>
-      <c r="F48" s="64" t="s">
+      <c r="F48" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="G48" s="66" t="s">
+      <c r="G48" s="46" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A49" s="48"/>
-      <c r="B49" s="62" t="s">
+      <c r="A49" s="77"/>
+      <c r="B49" s="42" t="s">
         <v>218</v>
       </c>
-      <c r="C49" s="63">
+      <c r="C49" s="43">
         <v>10</v>
       </c>
-      <c r="D49" s="63">
+      <c r="D49" s="43">
         <v>10</v>
       </c>
-      <c r="E49" s="63">
+      <c r="E49" s="43">
         <v>10</v>
       </c>
-      <c r="F49" s="64" t="s">
+      <c r="F49" s="44" t="s">
         <v>219</v>
       </c>
-      <c r="G49" s="66" t="s">
+      <c r="G49" s="46" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="49" t="s">
+      <c r="A50" s="60" t="s">
         <v>36</v>
       </c>
       <c r="B50" s="14" t="s">
@@ -2907,7 +2925,7 @@
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A51" s="50"/>
+      <c r="A51" s="61"/>
       <c r="B51" s="14" t="s">
         <v>26</v>
       </c>
@@ -2930,7 +2948,7 @@
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A52" s="50"/>
+      <c r="A52" s="61"/>
       <c r="B52" s="14" t="s">
         <v>27</v>
       </c>
@@ -2953,7 +2971,7 @@
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A53" s="50"/>
+      <c r="A53" s="61"/>
       <c r="B53" s="14" t="s">
         <v>28</v>
       </c>
@@ -2976,7 +2994,7 @@
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A54" s="50"/>
+      <c r="A54" s="61"/>
       <c r="B54" s="14" t="s">
         <v>29</v>
       </c>
@@ -2999,7 +3017,7 @@
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A55" s="50"/>
+      <c r="A55" s="61"/>
       <c r="B55" s="14" t="s">
         <v>30</v>
       </c>
@@ -3022,7 +3040,7 @@
       </c>
     </row>
     <row r="56" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="53" t="s">
+      <c r="A56" s="62" t="s">
         <v>33</v>
       </c>
       <c r="B56" s="17" t="s">
@@ -3049,7 +3067,7 @@
       <c r="L56" s="13"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A57" s="54"/>
+      <c r="A57" s="63"/>
       <c r="B57" s="17" t="s">
         <v>232</v>
       </c>
@@ -3058,11 +3076,11 @@
         <v>0.47222222222222221</v>
       </c>
       <c r="D57" s="18">
-        <f t="shared" ref="D57:D64" si="10">C57*0.8</f>
+        <f t="shared" ref="D57:D62" si="10">C57*0.8</f>
         <v>0.37777777777777777</v>
       </c>
       <c r="E57" s="18">
-        <f t="shared" ref="E57:E64" si="11">C57*1.2</f>
+        <f t="shared" ref="E57:E62" si="11">C57*1.2</f>
         <v>0.56666666666666665</v>
       </c>
       <c r="F57" s="19" t="s">
@@ -3074,7 +3092,7 @@
       <c r="L57" s="13"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A58" s="54"/>
+      <c r="A58" s="63"/>
       <c r="B58" s="17" t="s">
         <v>233</v>
       </c>
@@ -3099,7 +3117,7 @@
       <c r="L58" s="13"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A59" s="54"/>
+      <c r="A59" s="63"/>
       <c r="B59" s="17" t="s">
         <v>235</v>
       </c>
@@ -3121,7 +3139,7 @@
       <c r="L59" s="13"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A60" s="54"/>
+      <c r="A60" s="63"/>
       <c r="B60" s="17" t="s">
         <v>237</v>
       </c>
@@ -3146,7 +3164,7 @@
       <c r="L60" s="13"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A61" s="54"/>
+      <c r="A61" s="63"/>
       <c r="B61" s="17" t="s">
         <v>240</v>
       </c>
@@ -3170,7 +3188,7 @@
       <c r="L61" s="13"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A62" s="54"/>
+      <c r="A62" s="63"/>
       <c r="B62" s="17" t="s">
         <v>242</v>
       </c>
@@ -3193,7 +3211,7 @@
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A63" s="54"/>
+      <c r="A63" s="63"/>
       <c r="B63" s="20" t="s">
         <v>244</v>
       </c>
@@ -3214,15 +3232,15 @@
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A64" s="54"/>
+      <c r="A64" s="63"/>
       <c r="B64" s="20" t="s">
         <v>118</v>
       </c>
       <c r="C64" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D64" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E64" s="18">
         <v>4</v>
@@ -3236,7 +3254,7 @@
       <c r="L64" s="13"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A65" s="54"/>
+      <c r="A65" s="63"/>
       <c r="B65" s="20" t="s">
         <v>247</v>
       </c>
@@ -3256,7 +3274,7 @@
       <c r="L65" s="13"/>
     </row>
     <row r="66" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="54"/>
+      <c r="A66" s="63"/>
       <c r="B66" s="17" t="s">
         <v>249</v>
       </c>
@@ -3281,7 +3299,7 @@
       <c r="L66" s="13"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A67" s="54"/>
+      <c r="A67" s="63"/>
       <c r="B67" s="17" t="s">
         <v>250</v>
       </c>
@@ -3306,7 +3324,7 @@
       <c r="L67" s="13"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A68" s="54"/>
+      <c r="A68" s="63"/>
       <c r="B68" s="17" t="s">
         <v>252</v>
       </c>
@@ -3331,7 +3349,7 @@
       <c r="L68" s="13"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A69" s="55"/>
+      <c r="A69" s="64"/>
       <c r="B69" s="17" t="s">
         <v>77</v>
       </c>
@@ -3356,337 +3374,390 @@
       <c r="L69" s="13"/>
     </row>
     <row r="70" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="37" t="s">
+      <c r="A70" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="B70" s="67" t="s">
+      <c r="B70" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="C70" s="68">
+      <c r="C70" s="48">
         <v>0.25</v>
       </c>
-      <c r="D70" s="68">
+      <c r="D70" s="48">
         <f>C70</f>
         <v>0.25</v>
       </c>
-      <c r="E70" s="68">
+      <c r="E70" s="48">
         <f>C70</f>
         <v>0.25</v>
       </c>
-      <c r="F70" s="69"/>
-      <c r="G70" s="69" t="s">
+      <c r="F70" s="49"/>
+      <c r="G70" s="49" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A71" s="38"/>
-      <c r="B71" s="67" t="s">
+      <c r="A71" s="59"/>
+      <c r="B71" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="C71" s="68">
+      <c r="C71" s="48">
         <v>0.2</v>
       </c>
-      <c r="D71" s="68">
-        <f t="shared" ref="D71:D84" si="12">C71</f>
+      <c r="D71" s="48">
+        <f t="shared" ref="D71:D85" si="12">C71</f>
         <v>0.2</v>
       </c>
-      <c r="E71" s="68">
-        <f t="shared" ref="E71:E84" si="13">C71</f>
+      <c r="E71" s="48">
+        <f t="shared" ref="E71:E85" si="13">C71</f>
         <v>0.2</v>
       </c>
-      <c r="F71" s="69"/>
-      <c r="G71" s="69" t="s">
+      <c r="F71" s="49"/>
+      <c r="G71" s="49" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A72" s="38"/>
-      <c r="B72" s="67" t="s">
+      <c r="A72" s="59"/>
+      <c r="B72" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="C72" s="68">
+      <c r="C72" s="48">
         <v>0.2</v>
       </c>
-      <c r="D72" s="68">
+      <c r="D72" s="48">
         <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
-      <c r="E72" s="68">
+      <c r="E72" s="48">
         <f t="shared" si="13"/>
         <v>0.2</v>
       </c>
-      <c r="F72" s="69"/>
-      <c r="G72" s="69" t="s">
+      <c r="F72" s="49"/>
+      <c r="G72" s="49" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A73" s="38"/>
-      <c r="B73" s="67" t="s">
+      <c r="A73" s="59"/>
+      <c r="B73" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="C73" s="70">
+      <c r="C73" s="50">
         <v>0.2</v>
       </c>
-      <c r="D73" s="68">
+      <c r="D73" s="48">
         <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
-      <c r="E73" s="68">
+      <c r="E73" s="48">
         <f t="shared" si="13"/>
         <v>0.2</v>
       </c>
-      <c r="F73" s="69"/>
-      <c r="G73" s="69" t="s">
+      <c r="F73" s="49"/>
+      <c r="G73" s="49" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A74" s="38"/>
-      <c r="B74" s="67" t="s">
+      <c r="A74" s="59"/>
+      <c r="B74" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C74" s="70">
+      <c r="C74" s="50">
         <v>0.5</v>
       </c>
-      <c r="D74" s="68">
+      <c r="D74" s="48">
         <f t="shared" si="12"/>
         <v>0.5</v>
       </c>
-      <c r="E74" s="68">
+      <c r="E74" s="48">
         <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
-      <c r="F74" s="69"/>
-      <c r="G74" s="69" t="s">
+      <c r="F74" s="49"/>
+      <c r="G74" s="49" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A75" s="38"/>
-      <c r="B75" s="67" t="s">
-        <v>44</v>
-      </c>
-      <c r="C75" s="70">
+      <c r="A75" s="59"/>
+      <c r="B75" s="47" t="s">
+        <v>279</v>
+      </c>
+      <c r="C75" s="50">
         <v>0.25</v>
       </c>
-      <c r="D75" s="68">
+      <c r="D75" s="48">
         <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
-      <c r="E75" s="68">
+      <c r="E75" s="48">
         <f t="shared" si="13"/>
         <v>0.25</v>
       </c>
-      <c r="F75" s="69"/>
-      <c r="G75" s="69" t="s">
-        <v>108</v>
+      <c r="F75" s="49"/>
+      <c r="G75" s="49" t="s">
+        <v>282</v>
       </c>
       <c r="L75" s="13"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A76" s="38"/>
-      <c r="B76" s="67" t="s">
-        <v>50</v>
-      </c>
-      <c r="C76" s="70">
+      <c r="A76" s="59"/>
+      <c r="B76" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C76" s="50">
         <v>0.1</v>
       </c>
-      <c r="D76" s="68">
+      <c r="D76" s="48">
         <f t="shared" si="12"/>
         <v>0.1</v>
       </c>
-      <c r="E76" s="68">
+      <c r="E76" s="48">
         <f t="shared" si="13"/>
         <v>0.1</v>
       </c>
-      <c r="F76" s="69"/>
-      <c r="G76" s="69" t="s">
-        <v>109</v>
+      <c r="F76" s="49"/>
+      <c r="G76" s="49" t="s">
+        <v>108</v>
       </c>
       <c r="L76" s="13"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A77" s="38"/>
-      <c r="B77" s="67" t="s">
-        <v>45</v>
-      </c>
-      <c r="C77" s="70">
+      <c r="A77" s="59"/>
+      <c r="B77" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="C77" s="50">
         <v>0.1</v>
       </c>
-      <c r="D77" s="68">
+      <c r="D77" s="48">
         <f t="shared" si="12"/>
         <v>0.1</v>
       </c>
-      <c r="E77" s="68">
+      <c r="E77" s="48">
         <f t="shared" si="13"/>
         <v>0.1</v>
       </c>
-      <c r="F77" s="69"/>
-      <c r="G77" s="69" t="s">
-        <v>110</v>
+      <c r="F77" s="49"/>
+      <c r="G77" s="49" t="s">
+        <v>109</v>
       </c>
       <c r="L77" s="13"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A78" s="38"/>
-      <c r="B78" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="C78" s="70">
+      <c r="A78" s="59"/>
+      <c r="B78" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C78" s="50">
         <v>0.1</v>
       </c>
-      <c r="D78" s="68">
+      <c r="D78" s="48">
         <f t="shared" si="12"/>
         <v>0.1</v>
       </c>
-      <c r="E78" s="68">
+      <c r="E78" s="48">
         <f t="shared" si="13"/>
         <v>0.1</v>
       </c>
-      <c r="F78" s="69"/>
-      <c r="G78" s="69" t="s">
-        <v>111</v>
+      <c r="F78" s="49"/>
+      <c r="G78" s="49" t="s">
+        <v>110</v>
       </c>
       <c r="L78" s="13"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A79" s="38"/>
-      <c r="B79" s="67" t="s">
-        <v>47</v>
-      </c>
-      <c r="C79" s="70">
+      <c r="A79" s="59"/>
+      <c r="B79" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="C79" s="50">
         <v>0.45</v>
       </c>
-      <c r="D79" s="68">
+      <c r="D79" s="48">
         <f t="shared" si="12"/>
         <v>0.45</v>
       </c>
-      <c r="E79" s="68">
+      <c r="E79" s="48">
         <f t="shared" si="13"/>
         <v>0.45</v>
       </c>
-      <c r="F79" s="69"/>
-      <c r="G79" s="69" t="s">
-        <v>112</v>
+      <c r="F79" s="49"/>
+      <c r="G79" s="49" t="s">
+        <v>111</v>
       </c>
       <c r="L79" s="13"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A80" s="38"/>
-      <c r="B80" s="67" t="s">
-        <v>48</v>
-      </c>
-      <c r="C80" s="70">
+      <c r="A80" s="59"/>
+      <c r="B80" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="C80" s="50">
         <v>0.5</v>
       </c>
-      <c r="D80" s="68">
+      <c r="D80" s="48">
         <f t="shared" si="12"/>
         <v>0.5</v>
       </c>
-      <c r="E80" s="68">
+      <c r="E80" s="48">
         <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
-      <c r="F80" s="69"/>
-      <c r="G80" s="69" t="s">
-        <v>113</v>
+      <c r="F80" s="49"/>
+      <c r="G80" s="49" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A81" s="38"/>
-      <c r="B81" s="67" t="s">
-        <v>51</v>
-      </c>
-      <c r="C81" s="68">
+      <c r="A81" s="59"/>
+      <c r="B81" s="47" t="s">
+        <v>280</v>
+      </c>
+      <c r="C81" s="48">
         <v>0.7</v>
       </c>
-      <c r="D81" s="68">
+      <c r="D81" s="48">
         <f t="shared" si="12"/>
         <v>0.7</v>
       </c>
-      <c r="E81" s="68">
+      <c r="E81" s="48">
         <f t="shared" si="13"/>
         <v>0.7</v>
       </c>
-      <c r="F81" s="69"/>
-      <c r="G81" s="69" t="s">
-        <v>114</v>
+      <c r="F81" s="49"/>
+      <c r="G81" s="49" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A82" s="38"/>
-      <c r="B82" s="67" t="s">
-        <v>52</v>
-      </c>
-      <c r="C82" s="68">
+      <c r="A82" s="59"/>
+      <c r="B82" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C82" s="48">
         <v>0.7</v>
       </c>
-      <c r="D82" s="68">
+      <c r="D82" s="48">
         <f t="shared" si="12"/>
         <v>0.7</v>
       </c>
-      <c r="E82" s="68">
+      <c r="E82" s="48">
         <f t="shared" si="13"/>
         <v>0.7</v>
       </c>
-      <c r="F82" s="69"/>
-      <c r="G82" s="69" t="s">
-        <v>115</v>
+      <c r="F82" s="49"/>
+      <c r="G82" s="49" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A83" s="38"/>
-      <c r="B83" s="67" t="s">
-        <v>53</v>
-      </c>
-      <c r="C83" s="68">
+      <c r="A83" s="59"/>
+      <c r="B83" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C83" s="48">
         <v>0.7</v>
       </c>
-      <c r="D83" s="68">
+      <c r="D83" s="48">
         <f t="shared" si="12"/>
         <v>0.7</v>
       </c>
-      <c r="E83" s="68">
+      <c r="E83" s="48">
         <f t="shared" si="13"/>
         <v>0.7</v>
       </c>
-      <c r="F83" s="69"/>
-      <c r="G83" s="69" t="s">
-        <v>116</v>
+      <c r="F83" s="49"/>
+      <c r="G83" s="49" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A84" s="38"/>
-      <c r="B84" s="67" t="s">
-        <v>54</v>
-      </c>
-      <c r="C84" s="68">
+      <c r="A84" s="59"/>
+      <c r="B84" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C84" s="48">
         <v>0.05</v>
       </c>
-      <c r="D84" s="68">
+      <c r="D84" s="48">
         <f t="shared" si="12"/>
         <v>0.05</v>
       </c>
-      <c r="E84" s="68">
+      <c r="E84" s="48">
         <f t="shared" si="13"/>
         <v>0.05</v>
       </c>
-      <c r="F84" s="69"/>
-      <c r="G84" s="69" t="s">
+      <c r="F84" s="49"/>
+      <c r="G84" s="49" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A85" s="59"/>
+      <c r="B85" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C85" s="48">
+        <v>0.2</v>
+      </c>
+      <c r="D85" s="48">
+        <f t="shared" si="12"/>
+        <v>0.2</v>
+      </c>
+      <c r="E85" s="48">
+        <f t="shared" si="13"/>
+        <v>0.2</v>
+      </c>
+      <c r="F85" s="49"/>
+      <c r="G85" s="49" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A86" s="59"/>
+      <c r="B86" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="C86" s="48">
+        <v>0.05</v>
+      </c>
+      <c r="D86" s="48">
+        <f t="shared" ref="D86:D87" si="14">C86</f>
+        <v>0.05</v>
+      </c>
+      <c r="E86" s="48">
+        <f t="shared" ref="E86:E87" si="15">C86</f>
+        <v>0.05</v>
+      </c>
+      <c r="F86" s="49"/>
+      <c r="G86" s="49" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B85" s="71"/>
-      <c r="C85" s="72"/>
-      <c r="D85" s="72"/>
-      <c r="E85" s="72"/>
-      <c r="F85" s="73"/>
-      <c r="G85" s="73"/>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="L86" s="13"/>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A87" s="59"/>
+      <c r="B87" s="47" t="s">
+        <v>281</v>
+      </c>
+      <c r="C87" s="48">
+        <v>0.05</v>
+      </c>
+      <c r="D87" s="48">
+        <f t="shared" si="14"/>
+        <v>0.05</v>
+      </c>
+      <c r="E87" s="48">
+        <f t="shared" si="15"/>
+        <v>0.05</v>
+      </c>
+      <c r="F87" s="49"/>
+      <c r="G87" s="49" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="104" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L104" s="13"/>
@@ -3735,9 +3806,9 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A70:A87"/>
     <mergeCell ref="A50:A55"/>
     <mergeCell ref="A56:A69"/>
-    <mergeCell ref="A70:A84"/>
     <mergeCell ref="A4:A18"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="A19:A21"/>
@@ -3772,14 +3843,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="67" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" s="29"/>
@@ -3810,7 +3881,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="65" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -3836,7 +3907,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="41"/>
+      <c r="A5" s="65"/>
       <c r="B5" s="8" t="s">
         <v>276</v>
       </c>
@@ -3860,7 +3931,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="41"/>
+      <c r="A6" s="65"/>
       <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
@@ -3881,7 +3952,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="41"/>
+      <c r="A7" s="65"/>
       <c r="B7" s="8" t="s">
         <v>205</v>
       </c>
@@ -3903,7 +3974,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="41"/>
+      <c r="A8" s="65"/>
       <c r="B8" s="8" t="s">
         <v>206</v>
       </c>
@@ -3926,7 +3997,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="41"/>
+      <c r="A9" s="65"/>
       <c r="B9" s="8" t="s">
         <v>207</v>
       </c>
@@ -3947,7 +4018,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="41"/>
+      <c r="A10" s="65"/>
       <c r="B10" s="8" t="s">
         <v>55</v>
       </c>
@@ -3970,7 +4041,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="41"/>
+      <c r="A11" s="65"/>
       <c r="B11" s="8" t="s">
         <v>214</v>
       </c>
@@ -3991,7 +4062,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="41"/>
+      <c r="A12" s="65"/>
       <c r="B12" s="8" t="s">
         <v>123</v>
       </c>
@@ -4012,7 +4083,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="41"/>
+      <c r="A13" s="65"/>
       <c r="B13" s="8" t="s">
         <v>208</v>
       </c>
@@ -4033,7 +4104,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="41"/>
+      <c r="A14" s="65"/>
       <c r="B14" s="8" t="s">
         <v>209</v>
       </c>
@@ -4054,7 +4125,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="41"/>
+      <c r="A15" s="65"/>
       <c r="B15" s="8" t="s">
         <v>210</v>
       </c>
@@ -4075,7 +4146,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="41"/>
+      <c r="A16" s="65"/>
       <c r="B16" s="8" t="s">
         <v>211</v>
       </c>
@@ -4096,7 +4167,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="41"/>
+      <c r="A17" s="65"/>
       <c r="B17" s="8" t="s">
         <v>212</v>
       </c>
@@ -4117,7 +4188,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="78"/>
+      <c r="A18" s="66"/>
       <c r="B18" s="8" t="s">
         <v>213</v>
       </c>
@@ -4138,105 +4209,105 @@
       </c>
     </row>
     <row r="19" spans="1:7" s="31" customFormat="1" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="80" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="74" t="s">
+      <c r="B19" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="75">
+      <c r="C19" s="55">
         <f>107087/500*C23</f>
         <v>107087</v>
       </c>
-      <c r="D19" s="75">
+      <c r="D19" s="55">
         <f>107087/500*D23</f>
         <v>85669.6</v>
       </c>
-      <c r="E19" s="75">
+      <c r="E19" s="55">
         <f>107087/500*E23</f>
         <v>128504.40000000001</v>
       </c>
-      <c r="F19" s="76" t="s">
+      <c r="F19" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="G19" s="76" t="s">
+      <c r="G19" s="56" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="43"/>
-      <c r="B20" s="74" t="s">
+      <c r="A20" s="81"/>
+      <c r="B20" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="75">
+      <c r="C20" s="55">
         <f>190/500*C23</f>
         <v>190</v>
       </c>
-      <c r="D20" s="75">
+      <c r="D20" s="55">
         <f t="shared" ref="D20:E20" si="4">190/500*D23</f>
         <v>152</v>
       </c>
-      <c r="E20" s="75">
+      <c r="E20" s="55">
         <f t="shared" si="4"/>
         <v>228</v>
       </c>
-      <c r="F20" s="76" t="s">
+      <c r="F20" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="G20" s="76" t="s">
+      <c r="G20" s="56" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="43"/>
-      <c r="B21" s="74" t="s">
+      <c r="A21" s="81"/>
+      <c r="B21" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="75">
+      <c r="C21" s="55">
         <f>3000/4/500*C23</f>
         <v>750</v>
       </c>
-      <c r="D21" s="75">
+      <c r="D21" s="55">
         <f t="shared" ref="D21:E21" si="5">3000/4/500*D23</f>
         <v>600</v>
       </c>
-      <c r="E21" s="75">
+      <c r="E21" s="55">
         <f t="shared" si="5"/>
         <v>900</v>
       </c>
-      <c r="F21" s="76" t="s">
+      <c r="F21" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="G21" s="76" t="s">
+      <c r="G21" s="56" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="51" t="s">
+      <c r="A22" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="59" t="s">
+      <c r="B22" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="77">
+      <c r="C22" s="57">
         <v>48</v>
       </c>
-      <c r="D22" s="77">
+      <c r="D22" s="57">
         <v>48</v>
       </c>
-      <c r="E22" s="77">
+      <c r="E22" s="57">
         <f>C22*1.2</f>
         <v>57.599999999999994</v>
       </c>
-      <c r="F22" s="61" t="s">
+      <c r="F22" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="G22" s="61" t="s">
+      <c r="G22" s="41" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="52"/>
+      <c r="A23" s="72"/>
       <c r="B23" s="22" t="s">
         <v>65</v>
       </c>
@@ -4259,7 +4330,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="52"/>
+      <c r="A24" s="72"/>
       <c r="B24" s="22" t="s">
         <v>263</v>
       </c>
@@ -4283,7 +4354,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="52"/>
+      <c r="A25" s="72"/>
       <c r="B25" s="22" t="s">
         <v>124</v>
       </c>
@@ -4307,53 +4378,53 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="52"/>
-      <c r="B26" s="59" t="s">
+      <c r="A26" s="72"/>
+      <c r="B26" s="39" t="s">
         <v>264</v>
       </c>
-      <c r="C26" s="60">
+      <c r="C26" s="40">
         <v>10</v>
       </c>
-      <c r="D26" s="60">
+      <c r="D26" s="40">
         <f>C26*0.4</f>
         <v>4</v>
       </c>
-      <c r="E26" s="60">
+      <c r="E26" s="40">
         <f>C26*1.6</f>
         <v>16</v>
       </c>
-      <c r="F26" s="61" t="s">
+      <c r="F26" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="G26" s="61" t="s">
+      <c r="G26" s="41" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="52"/>
-      <c r="B27" s="59" t="s">
+      <c r="A27" s="72"/>
+      <c r="B27" s="39" t="s">
         <v>265</v>
       </c>
-      <c r="C27" s="60">
+      <c r="C27" s="40">
         <v>10</v>
       </c>
-      <c r="D27" s="60">
+      <c r="D27" s="40">
         <f>C27*0.4</f>
         <v>4</v>
       </c>
-      <c r="E27" s="60">
+      <c r="E27" s="40">
         <f>C27*1.6</f>
         <v>16</v>
       </c>
-      <c r="F27" s="61" t="s">
+      <c r="F27" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="G27" s="61" t="s">
+      <c r="G27" s="41" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="52"/>
+      <c r="A28" s="72"/>
       <c r="B28" s="22" t="s">
         <v>71</v>
       </c>
@@ -4376,7 +4447,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="52"/>
+      <c r="A29" s="72"/>
       <c r="B29" s="22" t="s">
         <v>72</v>
       </c>
@@ -4399,7 +4470,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="52"/>
+      <c r="A30" s="72"/>
       <c r="B30" s="22" t="s">
         <v>75</v>
       </c>
@@ -4422,7 +4493,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="44" t="s">
+      <c r="A31" s="73" t="s">
         <v>34</v>
       </c>
       <c r="B31" s="9" t="s">
@@ -4445,7 +4516,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="45"/>
+      <c r="A32" s="74"/>
       <c r="B32" s="9" t="s">
         <v>12</v>
       </c>
@@ -4466,7 +4537,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="45"/>
+      <c r="A33" s="74"/>
       <c r="B33" s="9" t="s">
         <v>222</v>
       </c>
@@ -4487,7 +4558,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="45"/>
+      <c r="A34" s="74"/>
       <c r="B34" s="9" t="s">
         <v>19</v>
       </c>
@@ -4508,7 +4579,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="45"/>
+      <c r="A35" s="74"/>
       <c r="B35" s="9" t="s">
         <v>13</v>
       </c>
@@ -4529,7 +4600,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="45"/>
+      <c r="A36" s="74"/>
       <c r="B36" s="9" t="s">
         <v>14</v>
       </c>
@@ -4550,7 +4621,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="45"/>
+      <c r="A37" s="74"/>
       <c r="B37" s="9" t="s">
         <v>15</v>
       </c>
@@ -4571,7 +4642,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="45"/>
+      <c r="A38" s="74"/>
       <c r="B38" s="9" t="s">
         <v>16</v>
       </c>
@@ -4592,7 +4663,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="45"/>
+      <c r="A39" s="74"/>
       <c r="B39" s="9" t="s">
         <v>226</v>
       </c>
@@ -4613,7 +4684,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="45"/>
+      <c r="A40" s="74"/>
       <c r="B40" s="9" t="s">
         <v>20</v>
       </c>
@@ -4634,7 +4705,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="45"/>
+      <c r="A41" s="74"/>
       <c r="B41" s="9" t="s">
         <v>17</v>
       </c>
@@ -4655,7 +4726,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="45"/>
+      <c r="A42" s="74"/>
       <c r="B42" s="9" t="s">
         <v>18</v>
       </c>
@@ -4676,171 +4747,171 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="46" t="s">
+      <c r="A43" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="62" t="s">
+      <c r="B43" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="C43" s="65">
+      <c r="C43" s="45">
         <v>100000</v>
       </c>
-      <c r="D43" s="65">
+      <c r="D43" s="45">
         <f t="shared" si="6"/>
         <v>80000</v>
       </c>
-      <c r="E43" s="65">
+      <c r="E43" s="45">
         <f t="shared" si="7"/>
         <v>120000</v>
       </c>
-      <c r="F43" s="64" t="s">
+      <c r="F43" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="G43" s="66" t="s">
+      <c r="G43" s="46" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="47"/>
-      <c r="B44" s="62" t="s">
+      <c r="A44" s="76"/>
+      <c r="B44" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="C44" s="65">
+      <c r="C44" s="45">
         <v>20000</v>
       </c>
-      <c r="D44" s="65">
+      <c r="D44" s="45">
         <f t="shared" si="6"/>
         <v>16000</v>
       </c>
-      <c r="E44" s="65">
+      <c r="E44" s="45">
         <f t="shared" si="7"/>
         <v>24000</v>
       </c>
-      <c r="F44" s="64" t="s">
+      <c r="F44" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="G44" s="66" t="s">
+      <c r="G44" s="46" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="47"/>
-      <c r="B45" s="62" t="s">
+      <c r="A45" s="76"/>
+      <c r="B45" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="C45" s="65">
+      <c r="C45" s="45">
         <v>40000</v>
       </c>
-      <c r="D45" s="65">
+      <c r="D45" s="45">
         <f t="shared" si="6"/>
         <v>32000</v>
       </c>
-      <c r="E45" s="65">
+      <c r="E45" s="45">
         <f t="shared" si="7"/>
         <v>48000</v>
       </c>
-      <c r="F45" s="64" t="s">
+      <c r="F45" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="G45" s="66" t="s">
+      <c r="G45" s="46" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="47"/>
-      <c r="B46" s="62" t="s">
+      <c r="A46" s="76"/>
+      <c r="B46" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="C46" s="63">
+      <c r="C46" s="43">
         <f>80/18000*(2*C24)</f>
         <v>169.44</v>
       </c>
-      <c r="D46" s="63">
+      <c r="D46" s="43">
         <f t="shared" si="6"/>
         <v>135.55199999999999</v>
       </c>
-      <c r="E46" s="63">
+      <c r="E46" s="43">
         <f t="shared" si="7"/>
         <v>203.328</v>
       </c>
-      <c r="F46" s="64" t="s">
+      <c r="F46" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="G46" s="66" t="s">
+      <c r="G46" s="46" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="47"/>
-      <c r="B47" s="62" t="s">
+      <c r="A47" s="76"/>
+      <c r="B47" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C47" s="63">
+      <c r="C47" s="43">
         <f>64/18000*(2*C24)</f>
         <v>135.55199999999999</v>
       </c>
-      <c r="D47" s="63">
+      <c r="D47" s="43">
         <f t="shared" si="6"/>
         <v>108.44159999999999</v>
       </c>
-      <c r="E47" s="63">
+      <c r="E47" s="43">
         <f t="shared" si="7"/>
         <v>162.66239999999999</v>
       </c>
-      <c r="F47" s="64" t="s">
+      <c r="F47" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="G47" s="66" t="s">
+      <c r="G47" s="46" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="47"/>
-      <c r="B48" s="62" t="s">
+      <c r="A48" s="76"/>
+      <c r="B48" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="C48" s="63">
+      <c r="C48" s="43">
         <f>(15+15+20+20+20+20+19+19+20+20+20+20+20+20)/1000/18000*(2*C24)</f>
         <v>0.56762400000000002</v>
       </c>
-      <c r="D48" s="63">
+      <c r="D48" s="43">
         <f t="shared" si="6"/>
         <v>0.45409920000000004</v>
       </c>
-      <c r="E48" s="63">
+      <c r="E48" s="43">
         <f t="shared" si="7"/>
         <v>0.6811488</v>
       </c>
-      <c r="F48" s="64" t="s">
+      <c r="F48" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="G48" s="66" t="s">
+      <c r="G48" s="46" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A49" s="48"/>
-      <c r="B49" s="62" t="s">
+      <c r="A49" s="77"/>
+      <c r="B49" s="42" t="s">
         <v>218</v>
       </c>
-      <c r="C49" s="63">
+      <c r="C49" s="43">
         <v>10</v>
       </c>
-      <c r="D49" s="63">
+      <c r="D49" s="43">
         <v>10</v>
       </c>
-      <c r="E49" s="63">
+      <c r="E49" s="43">
         <v>10</v>
       </c>
-      <c r="F49" s="64" t="s">
+      <c r="F49" s="44" t="s">
         <v>219</v>
       </c>
-      <c r="G49" s="66" t="s">
+      <c r="G49" s="46" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="49" t="s">
+      <c r="A50" s="60" t="s">
         <v>36</v>
       </c>
       <c r="B50" s="14" t="s">
@@ -4865,7 +4936,7 @@
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A51" s="50"/>
+      <c r="A51" s="61"/>
       <c r="B51" s="14" t="s">
         <v>26</v>
       </c>
@@ -4888,7 +4959,7 @@
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A52" s="50"/>
+      <c r="A52" s="61"/>
       <c r="B52" s="14" t="s">
         <v>27</v>
       </c>
@@ -4911,7 +4982,7 @@
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A53" s="50"/>
+      <c r="A53" s="61"/>
       <c r="B53" s="14" t="s">
         <v>28</v>
       </c>
@@ -4934,7 +5005,7 @@
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A54" s="50"/>
+      <c r="A54" s="61"/>
       <c r="B54" s="14" t="s">
         <v>29</v>
       </c>
@@ -4957,7 +5028,7 @@
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A55" s="50"/>
+      <c r="A55" s="61"/>
       <c r="B55" s="14" t="s">
         <v>30</v>
       </c>
@@ -4980,7 +5051,7 @@
       </c>
     </row>
     <row r="56" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="53" t="s">
+      <c r="A56" s="62" t="s">
         <v>33</v>
       </c>
       <c r="B56" s="17" t="s">
@@ -5007,7 +5078,7 @@
       <c r="L56" s="13"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A57" s="54"/>
+      <c r="A57" s="63"/>
       <c r="B57" s="17" t="s">
         <v>232</v>
       </c>
@@ -5016,11 +5087,11 @@
         <v>0.47222222222222221</v>
       </c>
       <c r="D57" s="18">
-        <f t="shared" ref="D57:D64" si="10">C57*0.8</f>
+        <f t="shared" ref="D57:D62" si="10">C57*0.8</f>
         <v>0.37777777777777777</v>
       </c>
       <c r="E57" s="18">
-        <f t="shared" ref="E57:E64" si="11">C57*1.2</f>
+        <f t="shared" ref="E57:E62" si="11">C57*1.2</f>
         <v>0.56666666666666665</v>
       </c>
       <c r="F57" s="19" t="s">
@@ -5032,7 +5103,7 @@
       <c r="L57" s="13"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A58" s="54"/>
+      <c r="A58" s="63"/>
       <c r="B58" s="17" t="s">
         <v>233</v>
       </c>
@@ -5057,7 +5128,7 @@
       <c r="L58" s="13"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A59" s="54"/>
+      <c r="A59" s="63"/>
       <c r="B59" s="17" t="s">
         <v>235</v>
       </c>
@@ -5079,7 +5150,7 @@
       <c r="L59" s="13"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A60" s="54"/>
+      <c r="A60" s="63"/>
       <c r="B60" s="17" t="s">
         <v>237</v>
       </c>
@@ -5104,7 +5175,7 @@
       <c r="L60" s="13"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A61" s="54"/>
+      <c r="A61" s="63"/>
       <c r="B61" s="17" t="s">
         <v>240</v>
       </c>
@@ -5128,7 +5199,7 @@
       <c r="L61" s="13"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A62" s="54"/>
+      <c r="A62" s="63"/>
       <c r="B62" s="17" t="s">
         <v>242</v>
       </c>
@@ -5151,7 +5222,7 @@
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A63" s="54"/>
+      <c r="A63" s="63"/>
       <c r="B63" s="20" t="s">
         <v>244</v>
       </c>
@@ -5172,7 +5243,7 @@
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A64" s="54"/>
+      <c r="A64" s="63"/>
       <c r="B64" s="20" t="s">
         <v>118</v>
       </c>
@@ -5194,7 +5265,7 @@
       <c r="L64" s="13"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A65" s="54"/>
+      <c r="A65" s="63"/>
       <c r="B65" s="20" t="s">
         <v>247</v>
       </c>
@@ -5214,7 +5285,7 @@
       <c r="L65" s="13"/>
     </row>
     <row r="66" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="54"/>
+      <c r="A66" s="63"/>
       <c r="B66" s="17" t="s">
         <v>249</v>
       </c>
@@ -5239,7 +5310,7 @@
       <c r="L66" s="13"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A67" s="54"/>
+      <c r="A67" s="63"/>
       <c r="B67" s="17" t="s">
         <v>250</v>
       </c>
@@ -5264,7 +5335,7 @@
       <c r="L67" s="13"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A68" s="54"/>
+      <c r="A68" s="63"/>
       <c r="B68" s="17" t="s">
         <v>252</v>
       </c>
@@ -5289,7 +5360,7 @@
       <c r="L68" s="13"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A69" s="55"/>
+      <c r="A69" s="64"/>
       <c r="B69" s="17" t="s">
         <v>77</v>
       </c>
@@ -5314,334 +5385,334 @@
       <c r="L69" s="13"/>
     </row>
     <row r="70" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="37" t="s">
+      <c r="A70" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="B70" s="67" t="s">
+      <c r="B70" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="C70" s="68">
+      <c r="C70" s="48">
         <v>0.25</v>
       </c>
-      <c r="D70" s="68">
+      <c r="D70" s="48">
         <f>C70</f>
         <v>0.25</v>
       </c>
-      <c r="E70" s="68">
+      <c r="E70" s="48">
         <f>C70</f>
         <v>0.25</v>
       </c>
-      <c r="F70" s="69"/>
-      <c r="G70" s="69" t="s">
+      <c r="F70" s="49"/>
+      <c r="G70" s="49" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A71" s="38"/>
-      <c r="B71" s="67" t="s">
+      <c r="A71" s="79"/>
+      <c r="B71" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="C71" s="68">
+      <c r="C71" s="48">
         <v>0.2</v>
       </c>
-      <c r="D71" s="68">
+      <c r="D71" s="48">
         <f t="shared" ref="D71:D84" si="12">C71</f>
         <v>0.2</v>
       </c>
-      <c r="E71" s="68">
+      <c r="E71" s="48">
         <f t="shared" ref="E71:E84" si="13">C71</f>
         <v>0.2</v>
       </c>
-      <c r="F71" s="69"/>
-      <c r="G71" s="69" t="s">
+      <c r="F71" s="49"/>
+      <c r="G71" s="49" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A72" s="38"/>
-      <c r="B72" s="67" t="s">
+      <c r="A72" s="79"/>
+      <c r="B72" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="C72" s="68">
+      <c r="C72" s="48">
         <v>0.2</v>
       </c>
-      <c r="D72" s="68">
+      <c r="D72" s="48">
         <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
-      <c r="E72" s="68">
+      <c r="E72" s="48">
         <f t="shared" si="13"/>
         <v>0.2</v>
       </c>
-      <c r="F72" s="69"/>
-      <c r="G72" s="69" t="s">
+      <c r="F72" s="49"/>
+      <c r="G72" s="49" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A73" s="38"/>
-      <c r="B73" s="67" t="s">
+      <c r="A73" s="79"/>
+      <c r="B73" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="C73" s="70">
+      <c r="C73" s="50">
         <v>0.2</v>
       </c>
-      <c r="D73" s="68">
+      <c r="D73" s="48">
         <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
-      <c r="E73" s="68">
+      <c r="E73" s="48">
         <f t="shared" si="13"/>
         <v>0.2</v>
       </c>
-      <c r="F73" s="69"/>
-      <c r="G73" s="69" t="s">
+      <c r="F73" s="49"/>
+      <c r="G73" s="49" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A74" s="38"/>
-      <c r="B74" s="67" t="s">
+      <c r="A74" s="79"/>
+      <c r="B74" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C74" s="70">
+      <c r="C74" s="50">
         <v>0.5</v>
       </c>
-      <c r="D74" s="68">
+      <c r="D74" s="48">
         <f t="shared" si="12"/>
         <v>0.5</v>
       </c>
-      <c r="E74" s="68">
+      <c r="E74" s="48">
         <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
-      <c r="F74" s="69"/>
-      <c r="G74" s="69" t="s">
+      <c r="F74" s="49"/>
+      <c r="G74" s="49" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A75" s="38"/>
-      <c r="B75" s="67" t="s">
+      <c r="A75" s="79"/>
+      <c r="B75" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="C75" s="70">
+      <c r="C75" s="50">
         <v>0.25</v>
       </c>
-      <c r="D75" s="68">
+      <c r="D75" s="48">
         <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
-      <c r="E75" s="68">
+      <c r="E75" s="48">
         <f t="shared" si="13"/>
         <v>0.25</v>
       </c>
-      <c r="F75" s="69"/>
-      <c r="G75" s="69" t="s">
+      <c r="F75" s="49"/>
+      <c r="G75" s="49" t="s">
         <v>108</v>
       </c>
       <c r="L75" s="13"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A76" s="38"/>
-      <c r="B76" s="67" t="s">
+      <c r="A76" s="79"/>
+      <c r="B76" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="C76" s="70">
+      <c r="C76" s="50">
         <v>0.1</v>
       </c>
-      <c r="D76" s="68">
+      <c r="D76" s="48">
         <f t="shared" si="12"/>
         <v>0.1</v>
       </c>
-      <c r="E76" s="68">
+      <c r="E76" s="48">
         <f t="shared" si="13"/>
         <v>0.1</v>
       </c>
-      <c r="F76" s="69"/>
-      <c r="G76" s="69" t="s">
+      <c r="F76" s="49"/>
+      <c r="G76" s="49" t="s">
         <v>109</v>
       </c>
       <c r="L76" s="13"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A77" s="38"/>
-      <c r="B77" s="67" t="s">
+      <c r="A77" s="79"/>
+      <c r="B77" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="C77" s="70">
+      <c r="C77" s="50">
         <v>0.1</v>
       </c>
-      <c r="D77" s="68">
+      <c r="D77" s="48">
         <f t="shared" si="12"/>
         <v>0.1</v>
       </c>
-      <c r="E77" s="68">
+      <c r="E77" s="48">
         <f t="shared" si="13"/>
         <v>0.1</v>
       </c>
-      <c r="F77" s="69"/>
-      <c r="G77" s="69" t="s">
+      <c r="F77" s="49"/>
+      <c r="G77" s="49" t="s">
         <v>110</v>
       </c>
       <c r="L77" s="13"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A78" s="38"/>
-      <c r="B78" s="67" t="s">
+      <c r="A78" s="79"/>
+      <c r="B78" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="C78" s="70">
+      <c r="C78" s="50">
         <v>0.1</v>
       </c>
-      <c r="D78" s="68">
+      <c r="D78" s="48">
         <f t="shared" si="12"/>
         <v>0.1</v>
       </c>
-      <c r="E78" s="68">
+      <c r="E78" s="48">
         <f t="shared" si="13"/>
         <v>0.1</v>
       </c>
-      <c r="F78" s="69"/>
-      <c r="G78" s="69" t="s">
+      <c r="F78" s="49"/>
+      <c r="G78" s="49" t="s">
         <v>111</v>
       </c>
       <c r="L78" s="13"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A79" s="38"/>
-      <c r="B79" s="67" t="s">
+      <c r="A79" s="79"/>
+      <c r="B79" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="C79" s="70">
+      <c r="C79" s="50">
         <v>0.45</v>
       </c>
-      <c r="D79" s="68">
+      <c r="D79" s="48">
         <f t="shared" si="12"/>
         <v>0.45</v>
       </c>
-      <c r="E79" s="68">
+      <c r="E79" s="48">
         <f t="shared" si="13"/>
         <v>0.45</v>
       </c>
-      <c r="F79" s="69"/>
-      <c r="G79" s="69" t="s">
+      <c r="F79" s="49"/>
+      <c r="G79" s="49" t="s">
         <v>112</v>
       </c>
       <c r="L79" s="13"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A80" s="38"/>
-      <c r="B80" s="67" t="s">
+      <c r="A80" s="79"/>
+      <c r="B80" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="C80" s="70">
+      <c r="C80" s="50">
         <v>0.5</v>
       </c>
-      <c r="D80" s="68">
+      <c r="D80" s="48">
         <f t="shared" si="12"/>
         <v>0.5</v>
       </c>
-      <c r="E80" s="68">
+      <c r="E80" s="48">
         <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
-      <c r="F80" s="69"/>
-      <c r="G80" s="69" t="s">
+      <c r="F80" s="49"/>
+      <c r="G80" s="49" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A81" s="38"/>
-      <c r="B81" s="67" t="s">
+      <c r="A81" s="79"/>
+      <c r="B81" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="C81" s="68">
+      <c r="C81" s="48">
         <v>0.7</v>
       </c>
-      <c r="D81" s="68">
+      <c r="D81" s="48">
         <f t="shared" si="12"/>
         <v>0.7</v>
       </c>
-      <c r="E81" s="68">
+      <c r="E81" s="48">
         <f t="shared" si="13"/>
         <v>0.7</v>
       </c>
-      <c r="F81" s="69"/>
-      <c r="G81" s="69" t="s">
+      <c r="F81" s="49"/>
+      <c r="G81" s="49" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A82" s="38"/>
-      <c r="B82" s="67" t="s">
+      <c r="A82" s="79"/>
+      <c r="B82" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="C82" s="68">
+      <c r="C82" s="48">
         <v>0.7</v>
       </c>
-      <c r="D82" s="68">
+      <c r="D82" s="48">
         <f t="shared" si="12"/>
         <v>0.7</v>
       </c>
-      <c r="E82" s="68">
+      <c r="E82" s="48">
         <f t="shared" si="13"/>
         <v>0.7</v>
       </c>
-      <c r="F82" s="69"/>
-      <c r="G82" s="69" t="s">
+      <c r="F82" s="49"/>
+      <c r="G82" s="49" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A83" s="38"/>
-      <c r="B83" s="67" t="s">
+      <c r="A83" s="79"/>
+      <c r="B83" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="C83" s="68">
+      <c r="C83" s="48">
         <v>0.7</v>
       </c>
-      <c r="D83" s="68">
+      <c r="D83" s="48">
         <f t="shared" si="12"/>
         <v>0.7</v>
       </c>
-      <c r="E83" s="68">
+      <c r="E83" s="48">
         <f t="shared" si="13"/>
         <v>0.7</v>
       </c>
-      <c r="F83" s="69"/>
-      <c r="G83" s="69" t="s">
+      <c r="F83" s="49"/>
+      <c r="G83" s="49" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A84" s="38"/>
-      <c r="B84" s="67" t="s">
+      <c r="A84" s="79"/>
+      <c r="B84" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="C84" s="68">
+      <c r="C84" s="48">
         <v>0.05</v>
       </c>
-      <c r="D84" s="68">
+      <c r="D84" s="48">
         <f t="shared" si="12"/>
         <v>0.05</v>
       </c>
-      <c r="E84" s="68">
+      <c r="E84" s="48">
         <f t="shared" si="13"/>
         <v>0.05</v>
       </c>
-      <c r="F84" s="69"/>
-      <c r="G84" s="69" t="s">
+      <c r="F84" s="49"/>
+      <c r="G84" s="49" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B85" s="71"/>
-      <c r="C85" s="72"/>
-      <c r="D85" s="72"/>
-      <c r="E85" s="72"/>
-      <c r="F85" s="73"/>
-      <c r="G85" s="73"/>
+      <c r="B85" s="51"/>
+      <c r="C85" s="52"/>
+      <c r="D85" s="52"/>
+      <c r="E85" s="52"/>
+      <c r="F85" s="53"/>
+      <c r="G85" s="53"/>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="L86" s="13"/>
@@ -5727,23 +5798,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="38" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="82" t="s">
         <v>145</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="E3" s="56" t="s">
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="E3" s="37" t="s">
         <v>147</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="G3" s="56" t="s">
+      <c r="G3" s="37" t="s">
         <v>148</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2o round of Antera
</commit_message>
<xml_diff>
--- a/Data/Antera_inputs.xlsx
+++ b/Data/Antera_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giparoli\Documents\Projetos\AEco\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB8A65E-EEE0-42BC-AA8F-1CD4E7545388}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17B9F70-888C-4702-A133-DC39F0BA9D14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Antera_spray" sheetId="8" r:id="rId1"/>
@@ -1108,6 +1108,36 @@
     <xf numFmtId="2" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1140,36 +1170,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1483,8 +1483,8 @@
   <dimension ref="A1:L129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B59" sqref="B59"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1499,14 +1499,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="63" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" s="28"/>
@@ -1537,7 +1537,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="61" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -1547,12 +1547,12 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D4" s="11">
-        <f>C4</f>
-        <v>1.0000000000000001E-5</v>
+        <f>C4*0.9</f>
+        <v>9.0000000000000002E-6</v>
       </c>
       <c r="E4" s="11">
-        <f>C4</f>
-        <v>1.0000000000000001E-5</v>
+        <f>C4*1.1</f>
+        <v>1.1000000000000001E-5</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>24</v>
@@ -1562,7 +1562,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1">
-      <c r="A5" s="72"/>
+      <c r="A5" s="61"/>
       <c r="B5" s="8" t="s">
         <v>188</v>
       </c>
@@ -1571,12 +1571,12 @@
         <v>0.5393258426966292</v>
       </c>
       <c r="D5" s="11">
-        <f t="shared" ref="D5:D68" si="0">C5</f>
-        <v>0.5393258426966292</v>
+        <f t="shared" ref="D5:D68" si="0">C5*0.9</f>
+        <v>0.48539325842696629</v>
       </c>
       <c r="E5" s="11">
-        <f t="shared" ref="E5:E18" si="1">C5</f>
-        <v>0.5393258426966292</v>
+        <f t="shared" ref="E5:E68" si="1">C5*1.1</f>
+        <v>0.59325842696629216</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>24</v>
@@ -1586,7 +1586,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="72"/>
+      <c r="A6" s="61"/>
       <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
@@ -1595,11 +1595,11 @@
       </c>
       <c r="D6" s="11">
         <f t="shared" si="0"/>
-        <v>563.97</v>
+        <v>507.57300000000004</v>
       </c>
       <c r="E6" s="11">
         <f t="shared" si="1"/>
-        <v>563.97</v>
+        <v>620.36700000000008</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>4</v>
@@ -1609,7 +1609,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="72"/>
+      <c r="A7" s="61"/>
       <c r="B7" s="8" t="s">
         <v>126</v>
       </c>
@@ -1618,11 +1618,11 @@
       </c>
       <c r="D7" s="11">
         <f t="shared" si="0"/>
-        <v>1028</v>
+        <v>925.2</v>
       </c>
       <c r="E7" s="11">
         <f t="shared" si="1"/>
-        <v>1028</v>
+        <v>1130.8000000000002</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>136</v>
@@ -1632,7 +1632,7 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="72"/>
+      <c r="A8" s="61"/>
       <c r="B8" s="8" t="s">
         <v>127</v>
       </c>
@@ -1642,11 +1642,11 @@
       </c>
       <c r="D8" s="11">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="E8" s="11">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>137</v>
@@ -1656,7 +1656,7 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="72"/>
+      <c r="A9" s="61"/>
       <c r="B9" s="8" t="s">
         <v>128</v>
       </c>
@@ -1665,11 +1665,11 @@
       </c>
       <c r="D9" s="11">
         <f t="shared" si="0"/>
-        <v>107</v>
+        <v>96.3</v>
       </c>
       <c r="E9" s="11">
         <f t="shared" si="1"/>
-        <v>107</v>
+        <v>117.7</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>125</v>
@@ -1679,7 +1679,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="72"/>
+      <c r="A10" s="61"/>
       <c r="B10" s="8" t="s">
         <v>54</v>
       </c>
@@ -1689,11 +1689,11 @@
       </c>
       <c r="D10" s="11">
         <f t="shared" si="0"/>
-        <v>30.666666666666668</v>
+        <v>27.6</v>
       </c>
       <c r="E10" s="11">
         <f t="shared" si="1"/>
-        <v>30.666666666666668</v>
+        <v>33.733333333333334</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>9</v>
@@ -1703,7 +1703,7 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="72"/>
+      <c r="A11" s="61"/>
       <c r="B11" s="8" t="s">
         <v>135</v>
       </c>
@@ -1712,11 +1712,11 @@
       </c>
       <c r="D11" s="11">
         <f t="shared" si="0"/>
-        <v>1.0000000000000001E-5</v>
+        <v>9.0000000000000002E-6</v>
       </c>
       <c r="E11" s="11">
         <f t="shared" si="1"/>
-        <v>1.0000000000000001E-5</v>
+        <v>1.1000000000000001E-5</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>6</v>
@@ -1726,7 +1726,7 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="72"/>
+      <c r="A12" s="61"/>
       <c r="B12" s="8" t="s">
         <v>122</v>
       </c>
@@ -1735,11 +1735,11 @@
       </c>
       <c r="D12" s="11">
         <f t="shared" si="0"/>
-        <v>8900</v>
+        <v>8010</v>
       </c>
       <c r="E12" s="11">
         <f t="shared" si="1"/>
-        <v>8900</v>
+        <v>9790</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>6</v>
@@ -1749,7 +1749,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="72"/>
+      <c r="A13" s="61"/>
       <c r="B13" s="8" t="s">
         <v>129</v>
       </c>
@@ -1758,11 +1758,11 @@
       </c>
       <c r="D13" s="11">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" s="11">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F13" s="31"/>
       <c r="G13" s="31" t="s">
@@ -1770,7 +1770,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="72"/>
+      <c r="A14" s="61"/>
       <c r="B14" s="8" t="s">
         <v>130</v>
       </c>
@@ -1779,11 +1779,11 @@
       </c>
       <c r="D14" s="11">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E14" s="11">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F14" s="31"/>
       <c r="G14" s="31" t="s">
@@ -1791,7 +1791,7 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="72"/>
+      <c r="A15" s="61"/>
       <c r="B15" s="8" t="s">
         <v>131</v>
       </c>
@@ -1800,11 +1800,11 @@
       </c>
       <c r="D15" s="11">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E15" s="11">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="F15" s="31"/>
       <c r="G15" s="31" t="s">
@@ -1812,7 +1812,7 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="72"/>
+      <c r="A16" s="61"/>
       <c r="B16" s="8" t="s">
         <v>132</v>
       </c>
@@ -1821,11 +1821,11 @@
       </c>
       <c r="D16" s="11">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" s="11">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F16" s="31"/>
       <c r="G16" s="31" t="s">
@@ -1833,7 +1833,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="72"/>
+      <c r="A17" s="61"/>
       <c r="B17" s="8" t="s">
         <v>133</v>
       </c>
@@ -1842,11 +1842,11 @@
       </c>
       <c r="D17" s="11">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E17" s="11">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F17" s="31"/>
       <c r="G17" s="31" t="s">
@@ -1854,7 +1854,7 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="73"/>
+      <c r="A18" s="62"/>
       <c r="B18" s="8" t="s">
         <v>134</v>
       </c>
@@ -1863,11 +1863,11 @@
       </c>
       <c r="D18" s="11">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E18" s="11">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="F18" s="31"/>
       <c r="G18" s="31" t="s">
@@ -1875,7 +1875,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" s="30" customFormat="1" ht="14.7" customHeight="1">
-      <c r="A19" s="55" t="s">
+      <c r="A19" s="65" t="s">
         <v>56</v>
       </c>
       <c r="B19" s="43" t="s">
@@ -1887,11 +1887,11 @@
       </c>
       <c r="D19" s="44">
         <f t="shared" si="0"/>
-        <v>510.43849999999998</v>
+        <v>459.39465000000001</v>
       </c>
       <c r="E19" s="44">
-        <f t="shared" ref="E19:E89" si="2">C19</f>
-        <v>510.43849999999998</v>
+        <f t="shared" si="1"/>
+        <v>561.48235</v>
       </c>
       <c r="F19" s="45" t="s">
         <v>55</v>
@@ -1901,7 +1901,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" s="30" customFormat="1">
-      <c r="A20" s="56"/>
+      <c r="A20" s="66"/>
       <c r="B20" s="43" t="s">
         <v>62</v>
       </c>
@@ -1911,11 +1911,11 @@
       </c>
       <c r="D20" s="44">
         <f t="shared" si="0"/>
-        <v>0.90566666666666662</v>
+        <v>0.81509999999999994</v>
       </c>
       <c r="E20" s="44">
-        <f t="shared" si="2"/>
-        <v>0.90566666666666662</v>
+        <f t="shared" si="1"/>
+        <v>0.99623333333333342</v>
       </c>
       <c r="F20" s="45" t="s">
         <v>69</v>
@@ -1925,7 +1925,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" s="30" customFormat="1">
-      <c r="A21" s="56"/>
+      <c r="A21" s="66"/>
       <c r="B21" s="43" t="s">
         <v>63</v>
       </c>
@@ -1935,11 +1935,11 @@
       </c>
       <c r="D21" s="44">
         <f t="shared" si="0"/>
-        <v>3.5750000000000002</v>
+        <v>3.2175000000000002</v>
       </c>
       <c r="E21" s="44">
-        <f t="shared" si="2"/>
-        <v>3.5750000000000002</v>
+        <f t="shared" si="1"/>
+        <v>3.9325000000000006</v>
       </c>
       <c r="F21" s="45" t="s">
         <v>69</v>
@@ -1949,7 +1949,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A22" s="57" t="s">
+      <c r="A22" s="67" t="s">
         <v>58</v>
       </c>
       <c r="B22" s="32" t="s">
@@ -1961,11 +1961,11 @@
       </c>
       <c r="D22" s="46">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E22" s="46">
-        <f t="shared" si="2"/>
-        <v>60</v>
+        <f t="shared" si="1"/>
+        <v>66</v>
       </c>
       <c r="F22" s="34" t="s">
         <v>61</v>
@@ -1975,7 +1975,7 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="58"/>
+      <c r="A23" s="68"/>
       <c r="B23" s="22" t="s">
         <v>64</v>
       </c>
@@ -1985,11 +1985,11 @@
       </c>
       <c r="D23" s="24">
         <f t="shared" si="0"/>
-        <v>2.3833333333333333</v>
+        <v>2.145</v>
       </c>
       <c r="E23" s="24">
-        <f t="shared" si="2"/>
-        <v>2.3833333333333333</v>
+        <f t="shared" si="1"/>
+        <v>2.621666666666667</v>
       </c>
       <c r="F23" s="23" t="s">
         <v>66</v>
@@ -1999,7 +1999,7 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="58"/>
+      <c r="A24" s="68"/>
       <c r="B24" s="22" t="s">
         <v>177</v>
       </c>
@@ -2008,11 +2008,11 @@
       </c>
       <c r="D24" s="24">
         <f t="shared" si="0"/>
-        <v>1.0000000000000001E-5</v>
+        <v>9.0000000000000002E-6</v>
       </c>
       <c r="E24" s="24">
-        <f t="shared" si="2"/>
-        <v>1.0000000000000001E-5</v>
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001E-5</v>
       </c>
       <c r="F24" s="23" t="s">
         <v>67</v>
@@ -2022,7 +2022,7 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="58"/>
+      <c r="A25" s="68"/>
       <c r="B25" s="22" t="s">
         <v>123</v>
       </c>
@@ -2031,11 +2031,11 @@
       </c>
       <c r="D25" s="24">
         <f t="shared" si="0"/>
-        <v>600</v>
+        <v>540</v>
       </c>
       <c r="E25" s="24">
-        <f t="shared" si="2"/>
-        <v>600</v>
+        <f t="shared" si="1"/>
+        <v>660</v>
       </c>
       <c r="F25" s="23" t="s">
         <v>67</v>
@@ -2045,7 +2045,7 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="58"/>
+      <c r="A26" s="68"/>
       <c r="B26" s="32" t="s">
         <v>178</v>
       </c>
@@ -2054,11 +2054,11 @@
       </c>
       <c r="D26" s="33">
         <f t="shared" si="0"/>
-        <v>1.0000000000000001E-5</v>
+        <v>9.0000000000000002E-6</v>
       </c>
       <c r="E26" s="33">
-        <f t="shared" si="2"/>
-        <v>1.0000000000000001E-5</v>
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001E-5</v>
       </c>
       <c r="F26" s="34" t="s">
         <v>68</v>
@@ -2068,7 +2068,7 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="58"/>
+      <c r="A27" s="68"/>
       <c r="B27" s="32" t="s">
         <v>179</v>
       </c>
@@ -2077,11 +2077,11 @@
       </c>
       <c r="D27" s="33">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5.4</v>
       </c>
       <c r="E27" s="33">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>6.6000000000000005</v>
       </c>
       <c r="F27" s="34" t="s">
         <v>68</v>
@@ -2091,7 +2091,7 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="58"/>
+      <c r="A28" s="68"/>
       <c r="B28" s="22" t="s">
         <v>70</v>
       </c>
@@ -2100,11 +2100,11 @@
       </c>
       <c r="D28" s="24">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="E28" s="24">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>3.3000000000000003</v>
       </c>
       <c r="F28" s="23" t="s">
         <v>68</v>
@@ -2114,7 +2114,7 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="58"/>
+      <c r="A29" s="68"/>
       <c r="B29" s="22" t="s">
         <v>71</v>
       </c>
@@ -2123,11 +2123,11 @@
       </c>
       <c r="D29" s="24">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E29" s="24">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F29" s="23" t="s">
         <v>68</v>
@@ -2137,7 +2137,7 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="58"/>
+      <c r="A30" s="68"/>
       <c r="B30" s="22" t="s">
         <v>74</v>
       </c>
@@ -2146,11 +2146,11 @@
       </c>
       <c r="D30" s="24">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="E30" s="24">
-        <f t="shared" si="2"/>
-        <v>1000</v>
+        <f t="shared" si="1"/>
+        <v>1100</v>
       </c>
       <c r="F30" s="23" t="s">
         <v>8</v>
@@ -2160,7 +2160,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A31" s="59" t="s">
+      <c r="A31" s="69" t="s">
         <v>34</v>
       </c>
       <c r="B31" s="9" t="s">
@@ -2171,11 +2171,11 @@
       </c>
       <c r="D31" s="12">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>1.8000000000000002E-2</v>
       </c>
       <c r="E31" s="12">
-        <f t="shared" si="2"/>
-        <v>0.02</v>
+        <f t="shared" si="1"/>
+        <v>2.2000000000000002E-2</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="7" t="s">
@@ -2183,7 +2183,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A32" s="60"/>
+      <c r="A32" s="70"/>
       <c r="B32" s="9" t="s">
         <v>12</v>
       </c>
@@ -2192,11 +2192,11 @@
       </c>
       <c r="D32" s="12">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.216</v>
       </c>
       <c r="E32" s="12">
-        <f t="shared" si="2"/>
-        <v>0.24</v>
+        <f t="shared" si="1"/>
+        <v>0.26400000000000001</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="7" t="s">
@@ -2204,7 +2204,7 @@
       </c>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="60"/>
+      <c r="A33" s="70"/>
       <c r="B33" s="9" t="s">
         <v>143</v>
       </c>
@@ -2213,11 +2213,11 @@
       </c>
       <c r="D33" s="12">
         <f t="shared" si="0"/>
-        <v>1.0000000000000001E-5</v>
+        <v>9.0000000000000002E-6</v>
       </c>
       <c r="E33" s="12">
-        <f t="shared" si="2"/>
-        <v>1.0000000000000001E-5</v>
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001E-5</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="7" t="s">
@@ -2225,7 +2225,7 @@
       </c>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="60"/>
+      <c r="A34" s="70"/>
       <c r="B34" s="9" t="s">
         <v>19</v>
       </c>
@@ -2234,11 +2234,11 @@
       </c>
       <c r="D34" s="12">
         <f t="shared" si="0"/>
-        <v>0.74</v>
+        <v>0.66600000000000004</v>
       </c>
       <c r="E34" s="12">
-        <f t="shared" si="2"/>
-        <v>0.74</v>
+        <f t="shared" si="1"/>
+        <v>0.81400000000000006</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="7" t="s">
@@ -2246,7 +2246,7 @@
       </c>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="60"/>
+      <c r="A35" s="70"/>
       <c r="B35" s="9" t="s">
         <v>13</v>
       </c>
@@ -2255,11 +2255,11 @@
       </c>
       <c r="D35" s="12">
         <f t="shared" si="0"/>
-        <v>1.0000000000000001E-5</v>
+        <v>9.0000000000000002E-6</v>
       </c>
       <c r="E35" s="12">
-        <f t="shared" si="2"/>
-        <v>1.0000000000000001E-5</v>
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001E-5</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="7" t="s">
@@ -2267,7 +2267,7 @@
       </c>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="60"/>
+      <c r="A36" s="70"/>
       <c r="B36" s="9" t="s">
         <v>14</v>
       </c>
@@ -2276,11 +2276,11 @@
       </c>
       <c r="D36" s="12">
         <f t="shared" si="0"/>
-        <v>1.0000000000000001E-5</v>
+        <v>9.0000000000000002E-6</v>
       </c>
       <c r="E36" s="12">
-        <f t="shared" si="2"/>
-        <v>1.0000000000000001E-5</v>
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001E-5</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="7" t="s">
@@ -2288,7 +2288,7 @@
       </c>
     </row>
     <row r="37" spans="1:12">
-      <c r="A37" s="60"/>
+      <c r="A37" s="70"/>
       <c r="B37" s="9" t="s">
         <v>15</v>
       </c>
@@ -2297,11 +2297,11 @@
       </c>
       <c r="D37" s="12">
         <f t="shared" si="0"/>
-        <v>1.25</v>
+        <v>1.125</v>
       </c>
       <c r="E37" s="12">
-        <f t="shared" si="2"/>
-        <v>1.25</v>
+        <f t="shared" si="1"/>
+        <v>1.375</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="7" t="s">
@@ -2309,7 +2309,7 @@
       </c>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="60"/>
+      <c r="A38" s="70"/>
       <c r="B38" s="9" t="s">
         <v>16</v>
       </c>
@@ -2318,11 +2318,11 @@
       </c>
       <c r="D38" s="12">
         <f t="shared" si="0"/>
-        <v>1.25</v>
+        <v>1.125</v>
       </c>
       <c r="E38" s="12">
-        <f t="shared" si="2"/>
-        <v>1.25</v>
+        <f t="shared" si="1"/>
+        <v>1.375</v>
       </c>
       <c r="F38" s="7"/>
       <c r="G38" s="7" t="s">
@@ -2330,7 +2330,7 @@
       </c>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="60"/>
+      <c r="A39" s="70"/>
       <c r="B39" s="9" t="s">
         <v>147</v>
       </c>
@@ -2339,11 +2339,11 @@
       </c>
       <c r="D39" s="12">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E39" s="12">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F39" s="7"/>
       <c r="G39" s="7" t="s">
@@ -2351,7 +2351,7 @@
       </c>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="60"/>
+      <c r="A40" s="70"/>
       <c r="B40" s="9" t="s">
         <v>20</v>
       </c>
@@ -2360,11 +2360,11 @@
       </c>
       <c r="D40" s="12">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>1.08</v>
       </c>
       <c r="E40" s="12">
-        <f t="shared" si="2"/>
-        <v>1.2</v>
+        <f t="shared" si="1"/>
+        <v>1.32</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="7" t="s">
@@ -2372,7 +2372,7 @@
       </c>
     </row>
     <row r="41" spans="1:12">
-      <c r="A41" s="60"/>
+      <c r="A41" s="70"/>
       <c r="B41" s="9" t="s">
         <v>17</v>
       </c>
@@ -2381,11 +2381,11 @@
       </c>
       <c r="D41" s="12">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E41" s="12">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="7" t="s">
@@ -2393,7 +2393,7 @@
       </c>
     </row>
     <row r="42" spans="1:12">
-      <c r="A42" s="60"/>
+      <c r="A42" s="70"/>
       <c r="B42" s="9" t="s">
         <v>18</v>
       </c>
@@ -2402,11 +2402,11 @@
       </c>
       <c r="D42" s="12">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E42" s="12">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F42" s="7"/>
       <c r="G42" s="7" t="s">
@@ -2414,7 +2414,7 @@
       </c>
     </row>
     <row r="43" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A43" s="61" t="s">
+      <c r="A43" s="71" t="s">
         <v>35</v>
       </c>
       <c r="B43" s="35" t="s">
@@ -2425,11 +2425,11 @@
       </c>
       <c r="D43" s="38">
         <f t="shared" si="0"/>
-        <v>1.0000000000000001E-5</v>
+        <v>9.0000000000000002E-6</v>
       </c>
       <c r="E43" s="38">
-        <f t="shared" si="2"/>
-        <v>1.0000000000000001E-5</v>
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001E-5</v>
       </c>
       <c r="F43" s="37" t="s">
         <v>55</v>
@@ -2439,7 +2439,7 @@
       </c>
     </row>
     <row r="44" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A44" s="62"/>
+      <c r="A44" s="72"/>
       <c r="B44" s="35" t="s">
         <v>120</v>
       </c>
@@ -2448,11 +2448,11 @@
       </c>
       <c r="D44" s="38">
         <f t="shared" si="0"/>
-        <v>1.0000000000000001E-5</v>
+        <v>9.0000000000000002E-6</v>
       </c>
       <c r="E44" s="38">
-        <f t="shared" si="2"/>
-        <v>1.0000000000000001E-5</v>
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001E-5</v>
       </c>
       <c r="F44" s="37" t="s">
         <v>55</v>
@@ -2462,7 +2462,7 @@
       </c>
     </row>
     <row r="45" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A45" s="62"/>
+      <c r="A45" s="72"/>
       <c r="B45" s="35" t="s">
         <v>121</v>
       </c>
@@ -2471,11 +2471,11 @@
       </c>
       <c r="D45" s="38">
         <f t="shared" si="0"/>
-        <v>1.0000000000000001E-5</v>
+        <v>9.0000000000000002E-6</v>
       </c>
       <c r="E45" s="38">
-        <f t="shared" si="2"/>
-        <v>1.0000000000000001E-5</v>
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001E-5</v>
       </c>
       <c r="F45" s="37" t="s">
         <v>55</v>
@@ -2485,7 +2485,7 @@
       </c>
     </row>
     <row r="46" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A46" s="62"/>
+      <c r="A46" s="72"/>
       <c r="B46" s="47" t="s">
         <v>197</v>
       </c>
@@ -2495,11 +2495,11 @@
       </c>
       <c r="D46" s="38">
         <f t="shared" si="0"/>
-        <v>2664.0000000000005</v>
+        <v>2397.6000000000004</v>
       </c>
       <c r="E46" s="38">
-        <f t="shared" ref="E46" si="3">C46</f>
-        <v>2664.0000000000005</v>
+        <f t="shared" si="1"/>
+        <v>2930.4000000000005</v>
       </c>
       <c r="F46" s="39" t="s">
         <v>55</v>
@@ -2508,14 +2508,14 @@
         <v>198</v>
       </c>
       <c r="H46" s="48"/>
-      <c r="J46" s="64" t="s">
+      <c r="J46" s="53" t="s">
         <v>199</v>
       </c>
-      <c r="K46" s="64"/>
-      <c r="L46" s="64"/>
+      <c r="K46" s="53"/>
+      <c r="L46" s="53"/>
     </row>
     <row r="47" spans="1:12">
-      <c r="A47" s="62"/>
+      <c r="A47" s="72"/>
       <c r="B47" s="35" t="s">
         <v>21</v>
       </c>
@@ -2525,11 +2525,11 @@
       </c>
       <c r="D47" s="36">
         <f t="shared" si="0"/>
-        <v>2.6640000000000001</v>
+        <v>2.3976000000000002</v>
       </c>
       <c r="E47" s="36">
-        <f t="shared" si="2"/>
-        <v>2.6640000000000001</v>
+        <f t="shared" si="1"/>
+        <v>2.9304000000000006</v>
       </c>
       <c r="F47" s="37" t="s">
         <v>69</v>
@@ -2539,7 +2539,7 @@
       </c>
     </row>
     <row r="48" spans="1:12">
-      <c r="A48" s="62"/>
+      <c r="A48" s="72"/>
       <c r="B48" s="35" t="s">
         <v>22</v>
       </c>
@@ -2549,11 +2549,11 @@
       </c>
       <c r="D48" s="36">
         <f t="shared" si="0"/>
-        <v>2.1359999999999997</v>
+        <v>1.9223999999999997</v>
       </c>
       <c r="E48" s="36">
-        <f t="shared" si="2"/>
-        <v>2.1359999999999997</v>
+        <f t="shared" si="1"/>
+        <v>2.3495999999999997</v>
       </c>
       <c r="F48" s="37" t="s">
         <v>69</v>
@@ -2563,7 +2563,7 @@
       </c>
     </row>
     <row r="49" spans="1:11">
-      <c r="A49" s="62"/>
+      <c r="A49" s="72"/>
       <c r="B49" s="35" t="s">
         <v>23</v>
       </c>
@@ -2573,11 +2573,11 @@
       </c>
       <c r="D49" s="36">
         <f t="shared" si="0"/>
-        <v>9.0000000000000011E-3</v>
+        <v>8.1000000000000013E-3</v>
       </c>
       <c r="E49" s="36">
-        <f t="shared" si="2"/>
-        <v>9.0000000000000011E-3</v>
+        <f t="shared" si="1"/>
+        <v>9.9000000000000025E-3</v>
       </c>
       <c r="F49" s="37" t="s">
         <v>69</v>
@@ -2587,7 +2587,7 @@
       </c>
     </row>
     <row r="50" spans="1:11">
-      <c r="A50" s="63"/>
+      <c r="A50" s="73"/>
       <c r="B50" s="35" t="s">
         <v>139</v>
       </c>
@@ -2596,11 +2596,11 @@
       </c>
       <c r="D50" s="36">
         <f t="shared" si="0"/>
-        <v>1.0000000000000001E-5</v>
+        <v>9.0000000000000002E-6</v>
       </c>
       <c r="E50" s="36">
-        <f t="shared" si="2"/>
-        <v>1.0000000000000001E-5</v>
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001E-5</v>
       </c>
       <c r="F50" s="37" t="s">
         <v>140</v>
@@ -2610,7 +2610,7 @@
       </c>
     </row>
     <row r="51" spans="1:11" ht="14.4" customHeight="1">
-      <c r="A51" s="70" t="s">
+      <c r="A51" s="59" t="s">
         <v>36</v>
       </c>
       <c r="B51" s="14" t="s">
@@ -2622,11 +2622,11 @@
       </c>
       <c r="D51" s="15">
         <f t="shared" si="0"/>
-        <v>240</v>
+        <v>216</v>
       </c>
       <c r="E51" s="15">
-        <f t="shared" si="2"/>
-        <v>240</v>
+        <f t="shared" si="1"/>
+        <v>264</v>
       </c>
       <c r="F51" s="16" t="s">
         <v>7</v>
@@ -2636,7 +2636,7 @@
       </c>
     </row>
     <row r="52" spans="1:11">
-      <c r="A52" s="71"/>
+      <c r="A52" s="60"/>
       <c r="B52" s="14" t="s">
         <v>26</v>
       </c>
@@ -2645,11 +2645,11 @@
       </c>
       <c r="D52" s="15">
         <f t="shared" si="0"/>
-        <v>1.0000000000000001E-5</v>
+        <v>9.0000000000000002E-6</v>
       </c>
       <c r="E52" s="15">
-        <f t="shared" si="2"/>
-        <v>1.0000000000000001E-5</v>
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001E-5</v>
       </c>
       <c r="F52" s="16" t="s">
         <v>7</v>
@@ -2659,7 +2659,7 @@
       </c>
     </row>
     <row r="53" spans="1:11">
-      <c r="A53" s="71"/>
+      <c r="A53" s="60"/>
       <c r="B53" s="14" t="s">
         <v>27</v>
       </c>
@@ -2669,11 +2669,11 @@
       </c>
       <c r="D53" s="15">
         <f t="shared" si="0"/>
-        <v>8936.2000000000007</v>
+        <v>8042.5800000000008</v>
       </c>
       <c r="E53" s="15">
-        <f t="shared" si="2"/>
-        <v>8936.2000000000007</v>
+        <f t="shared" si="1"/>
+        <v>9829.8200000000015</v>
       </c>
       <c r="F53" s="16" t="s">
         <v>7</v>
@@ -2683,7 +2683,7 @@
       </c>
     </row>
     <row r="54" spans="1:11">
-      <c r="A54" s="71"/>
+      <c r="A54" s="60"/>
       <c r="B54" s="14" t="s">
         <v>28</v>
       </c>
@@ -2693,11 +2693,11 @@
       </c>
       <c r="D54" s="15">
         <f t="shared" si="0"/>
-        <v>0.56397000000000008</v>
+        <v>0.50757300000000005</v>
       </c>
       <c r="E54" s="15">
-        <f t="shared" si="2"/>
-        <v>0.56397000000000008</v>
+        <f t="shared" si="1"/>
+        <v>0.62036700000000011</v>
       </c>
       <c r="F54" s="16" t="s">
         <v>31</v>
@@ -2707,7 +2707,7 @@
       </c>
     </row>
     <row r="55" spans="1:11">
-      <c r="A55" s="71"/>
+      <c r="A55" s="60"/>
       <c r="B55" s="14" t="s">
         <v>29</v>
       </c>
@@ -2716,11 +2716,11 @@
       </c>
       <c r="D55" s="15">
         <f t="shared" si="0"/>
-        <v>1.0000000000000001E-5</v>
+        <v>9.0000000000000002E-6</v>
       </c>
       <c r="E55" s="15">
-        <f t="shared" si="2"/>
-        <v>1.0000000000000001E-5</v>
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001E-5</v>
       </c>
       <c r="F55" s="16" t="s">
         <v>31</v>
@@ -2730,7 +2730,7 @@
       </c>
     </row>
     <row r="56" spans="1:11">
-      <c r="A56" s="71"/>
+      <c r="A56" s="60"/>
       <c r="B56" s="14" t="s">
         <v>30</v>
       </c>
@@ -2740,11 +2740,11 @@
       </c>
       <c r="D56" s="15">
         <f t="shared" si="0"/>
-        <v>0.39477900000000005</v>
+        <v>0.35530110000000004</v>
       </c>
       <c r="E56" s="15">
-        <f t="shared" si="2"/>
-        <v>0.39477900000000005</v>
+        <f t="shared" si="1"/>
+        <v>0.43425690000000011</v>
       </c>
       <c r="F56" s="16" t="s">
         <v>31</v>
@@ -2754,7 +2754,7 @@
       </c>
     </row>
     <row r="57" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A57" s="65" t="s">
+      <c r="A57" s="54" t="s">
         <v>33</v>
       </c>
       <c r="B57" s="17" t="s">
@@ -2765,11 +2765,11 @@
       </c>
       <c r="D57" s="25">
         <f t="shared" si="0"/>
-        <v>8.8198500000000006E-3</v>
+        <v>7.9378650000000005E-3</v>
       </c>
       <c r="E57" s="25">
-        <f t="shared" ref="E57:E76" si="4">C57</f>
-        <v>8.8198500000000006E-3</v>
+        <f t="shared" si="1"/>
+        <v>9.7018350000000007E-3</v>
       </c>
       <c r="F57" s="19" t="s">
         <v>10</v>
@@ -2780,7 +2780,7 @@
       <c r="K57" s="13"/>
     </row>
     <row r="58" spans="1:11">
-      <c r="A58" s="66"/>
+      <c r="A58" s="55"/>
       <c r="B58" s="17" t="s">
         <v>153</v>
       </c>
@@ -2789,11 +2789,11 @@
       </c>
       <c r="D58" s="18">
         <f t="shared" si="0"/>
-        <v>1.04578E-2</v>
+        <v>9.4120200000000001E-3</v>
       </c>
       <c r="E58" s="18">
-        <f t="shared" si="4"/>
-        <v>1.04578E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.1503580000000001E-2</v>
       </c>
       <c r="F58" s="19" t="s">
         <v>10</v>
@@ -2804,7 +2804,7 @@
       <c r="K58" s="13"/>
     </row>
     <row r="59" spans="1:11">
-      <c r="A59" s="66"/>
+      <c r="A59" s="55"/>
       <c r="B59" s="17" t="s">
         <v>201</v>
       </c>
@@ -2814,11 +2814,11 @@
       </c>
       <c r="D59" s="18">
         <f t="shared" si="0"/>
-        <v>4.4099300000000003E-3</v>
+        <v>3.9689370000000005E-3</v>
       </c>
       <c r="E59" s="18">
-        <f t="shared" si="4"/>
-        <v>4.4099300000000003E-3</v>
+        <f t="shared" si="1"/>
+        <v>4.8509230000000009E-3</v>
       </c>
       <c r="F59" s="19" t="s">
         <v>10</v>
@@ -2829,7 +2829,7 @@
       <c r="K59" s="13"/>
     </row>
     <row r="60" spans="1:11">
-      <c r="A60" s="66"/>
+      <c r="A60" s="55"/>
       <c r="B60" s="17" t="s">
         <v>202</v>
       </c>
@@ -2839,18 +2839,18 @@
       </c>
       <c r="D60" s="18">
         <f t="shared" si="0"/>
-        <v>9.5758400000000004E-3</v>
+        <v>8.6182560000000012E-3</v>
       </c>
       <c r="E60" s="18">
-        <f t="shared" si="4"/>
-        <v>9.5758400000000004E-3</v>
+        <f t="shared" si="1"/>
+        <v>1.0533424000000001E-2</v>
       </c>
       <c r="F60" s="19"/>
       <c r="G60" s="19"/>
       <c r="K60" s="13"/>
     </row>
     <row r="61" spans="1:11">
-      <c r="A61" s="66"/>
+      <c r="A61" s="55"/>
       <c r="B61" s="17" t="s">
         <v>203</v>
       </c>
@@ -2860,18 +2860,18 @@
       </c>
       <c r="D61" s="18">
         <f t="shared" si="0"/>
-        <v>9.4498399999999993E-3</v>
+        <v>8.5048559999999999E-3</v>
       </c>
       <c r="E61" s="18">
-        <f t="shared" si="4"/>
-        <v>9.4498399999999993E-3</v>
+        <f t="shared" si="1"/>
+        <v>1.0394824E-2</v>
       </c>
       <c r="F61" s="19"/>
       <c r="G61" s="19"/>
       <c r="K61" s="13"/>
     </row>
     <row r="62" spans="1:11">
-      <c r="A62" s="66"/>
+      <c r="A62" s="55"/>
       <c r="B62" s="17" t="s">
         <v>155</v>
       </c>
@@ -2881,11 +2881,11 @@
       </c>
       <c r="D62" s="18">
         <f t="shared" si="0"/>
-        <v>379.20000000000005</v>
+        <v>341.28000000000003</v>
       </c>
       <c r="E62" s="18">
-        <f t="shared" si="4"/>
-        <v>379.20000000000005</v>
+        <f t="shared" si="1"/>
+        <v>417.12000000000006</v>
       </c>
       <c r="F62" s="19" t="s">
         <v>156</v>
@@ -2896,7 +2896,7 @@
       <c r="K62" s="13"/>
     </row>
     <row r="63" spans="1:11">
-      <c r="A63" s="66"/>
+      <c r="A63" s="55"/>
       <c r="B63" s="17" t="s">
         <v>158</v>
       </c>
@@ -2906,11 +2906,11 @@
       </c>
       <c r="D63" s="18">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>29.7</v>
       </c>
       <c r="E63" s="18">
-        <f t="shared" si="4"/>
-        <v>33</v>
+        <f t="shared" si="1"/>
+        <v>36.300000000000004</v>
       </c>
       <c r="F63" s="19" t="s">
         <v>156</v>
@@ -2921,7 +2921,7 @@
       <c r="K63" s="13"/>
     </row>
     <row r="64" spans="1:11">
-      <c r="A64" s="66"/>
+      <c r="A64" s="55"/>
       <c r="B64" s="20" t="s">
         <v>204</v>
       </c>
@@ -2931,11 +2931,11 @@
       </c>
       <c r="D64" s="18">
         <f t="shared" si="0"/>
-        <v>162</v>
+        <v>145.80000000000001</v>
       </c>
       <c r="E64" s="18">
-        <f t="shared" si="4"/>
-        <v>162</v>
+        <f t="shared" si="1"/>
+        <v>178.20000000000002</v>
       </c>
       <c r="F64" s="19" t="s">
         <v>156</v>
@@ -2945,7 +2945,7 @@
       </c>
     </row>
     <row r="65" spans="1:11">
-      <c r="A65" s="66"/>
+      <c r="A65" s="55"/>
       <c r="B65" s="20" t="s">
         <v>205</v>
       </c>
@@ -2955,17 +2955,17 @@
       </c>
       <c r="D65" s="18">
         <f t="shared" si="0"/>
-        <v>312</v>
+        <v>280.8</v>
       </c>
       <c r="E65" s="18">
-        <f t="shared" si="4"/>
-        <v>312</v>
+        <f t="shared" si="1"/>
+        <v>343.20000000000005</v>
       </c>
       <c r="F65" s="21"/>
       <c r="G65" s="19"/>
     </row>
     <row r="66" spans="1:11">
-      <c r="A66" s="66"/>
+      <c r="A66" s="55"/>
       <c r="B66" s="20" t="s">
         <v>206</v>
       </c>
@@ -2975,17 +2975,17 @@
       </c>
       <c r="D66" s="18">
         <f t="shared" si="0"/>
-        <v>169.2</v>
+        <v>152.28</v>
       </c>
       <c r="E66" s="18">
-        <f t="shared" si="4"/>
-        <v>169.2</v>
+        <f t="shared" si="1"/>
+        <v>186.12</v>
       </c>
       <c r="F66" s="21"/>
       <c r="G66" s="19"/>
     </row>
     <row r="67" spans="1:11">
-      <c r="A67" s="66"/>
+      <c r="A67" s="55"/>
       <c r="B67" s="20" t="s">
         <v>117</v>
       </c>
@@ -2994,11 +2994,11 @@
       </c>
       <c r="D67" s="18">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="E67" s="18">
-        <f t="shared" si="4"/>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F67" s="21" t="s">
         <v>124</v>
@@ -3009,7 +3009,7 @@
       <c r="K67" s="13"/>
     </row>
     <row r="68" spans="1:11">
-      <c r="A68" s="66"/>
+      <c r="A68" s="55"/>
       <c r="B68" s="20" t="s">
         <v>207</v>
       </c>
@@ -3019,11 +3019,11 @@
       </c>
       <c r="D68" s="18">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="E68" s="18">
-        <f t="shared" si="4"/>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F68" s="21" t="s">
         <v>124</v>
@@ -3032,7 +3032,7 @@
       <c r="K68" s="13"/>
     </row>
     <row r="69" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A69" s="66"/>
+      <c r="A69" s="55"/>
       <c r="B69" s="20" t="s">
         <v>162</v>
       </c>
@@ -3040,12 +3040,12 @@
         <v>0.95</v>
       </c>
       <c r="D69" s="18">
-        <f t="shared" ref="D69:D76" si="5">C69</f>
-        <v>0.95</v>
+        <f t="shared" ref="D69:D94" si="2">C69*0.9</f>
+        <v>0.85499999999999998</v>
       </c>
       <c r="E69" s="18">
-        <f t="shared" si="4"/>
-        <v>0.95</v>
+        <f t="shared" ref="E69:E94" si="3">C69*1.1</f>
+        <v>1.0449999999999999</v>
       </c>
       <c r="F69" s="21"/>
       <c r="G69" s="19" t="s">
@@ -3054,7 +3054,7 @@
       <c r="K69" s="13"/>
     </row>
     <row r="70" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A70" s="66"/>
+      <c r="A70" s="55"/>
       <c r="B70" s="20" t="s">
         <v>208</v>
       </c>
@@ -3062,19 +3062,19 @@
         <v>1</v>
       </c>
       <c r="D70" s="18">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0.9</v>
       </c>
       <c r="E70" s="18">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F70" s="21"/>
       <c r="G70" s="19"/>
       <c r="K70" s="13"/>
     </row>
     <row r="71" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A71" s="66"/>
+      <c r="A71" s="55"/>
       <c r="B71" s="20" t="s">
         <v>210</v>
       </c>
@@ -3082,12 +3082,12 @@
         <v>10</v>
       </c>
       <c r="D71" s="18">
-        <f t="shared" si="5"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="E71" s="18">
-        <f t="shared" si="4"/>
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>11</v>
       </c>
       <c r="F71" s="21" t="s">
         <v>209</v>
@@ -3098,7 +3098,7 @@
       <c r="K71" s="13"/>
     </row>
     <row r="72" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A72" s="66"/>
+      <c r="A72" s="55"/>
       <c r="B72" s="20" t="s">
         <v>211</v>
       </c>
@@ -3107,12 +3107,12 @@
         <v>75</v>
       </c>
       <c r="D72" s="18">
-        <f t="shared" si="5"/>
-        <v>75</v>
+        <f t="shared" si="2"/>
+        <v>67.5</v>
       </c>
       <c r="E72" s="18">
-        <f t="shared" si="4"/>
-        <v>75</v>
+        <f t="shared" si="3"/>
+        <v>82.5</v>
       </c>
       <c r="F72" s="21" t="s">
         <v>209</v>
@@ -3121,7 +3121,7 @@
       <c r="K72" s="13"/>
     </row>
     <row r="73" spans="1:11" ht="14.55" customHeight="1">
-      <c r="A73" s="66"/>
+      <c r="A73" s="55"/>
       <c r="B73" s="17" t="s">
         <v>164</v>
       </c>
@@ -3129,12 +3129,12 @@
         <v>2.3315789473684214</v>
       </c>
       <c r="D73" s="18">
-        <f t="shared" si="5"/>
-        <v>2.3315789473684214</v>
+        <f t="shared" si="2"/>
+        <v>2.0984210526315792</v>
       </c>
       <c r="E73" s="18">
-        <f t="shared" si="4"/>
-        <v>2.3315789473684214</v>
+        <f t="shared" si="3"/>
+        <v>2.5647368421052636</v>
       </c>
       <c r="F73" s="19" t="s">
         <v>32</v>
@@ -3145,7 +3145,7 @@
       <c r="K73" s="13"/>
     </row>
     <row r="74" spans="1:11">
-      <c r="A74" s="66"/>
+      <c r="A74" s="55"/>
       <c r="B74" s="17" t="s">
         <v>165</v>
       </c>
@@ -3153,12 +3153,12 @@
         <v>4.4784688995215309E-2</v>
       </c>
       <c r="D74" s="18">
-        <f t="shared" si="5"/>
-        <v>4.4784688995215309E-2</v>
+        <f t="shared" si="2"/>
+        <v>4.0306220095693776E-2</v>
       </c>
       <c r="E74" s="18">
-        <f t="shared" si="4"/>
-        <v>4.4784688995215309E-2</v>
+        <f t="shared" si="3"/>
+        <v>4.9263157894736842E-2</v>
       </c>
       <c r="F74" s="19" t="s">
         <v>32</v>
@@ -3169,7 +3169,7 @@
       <c r="K74" s="13"/>
     </row>
     <row r="75" spans="1:11">
-      <c r="A75" s="66"/>
+      <c r="A75" s="55"/>
       <c r="B75" s="17" t="s">
         <v>167</v>
       </c>
@@ -3177,12 +3177,12 @@
         <v>4.2497607655502394</v>
       </c>
       <c r="D75" s="18">
-        <f t="shared" si="5"/>
-        <v>4.2497607655502394</v>
+        <f t="shared" si="2"/>
+        <v>3.8247846889952157</v>
       </c>
       <c r="E75" s="18">
-        <f t="shared" si="4"/>
-        <v>4.2497607655502394</v>
+        <f t="shared" si="3"/>
+        <v>4.674736842105264</v>
       </c>
       <c r="F75" s="19" t="s">
         <v>32</v>
@@ -3193,7 +3193,7 @@
       <c r="K75" s="13"/>
     </row>
     <row r="76" spans="1:11">
-      <c r="A76" s="67"/>
+      <c r="A76" s="56"/>
       <c r="B76" s="17" t="s">
         <v>76</v>
       </c>
@@ -3201,12 +3201,12 @@
         <v>6</v>
       </c>
       <c r="D76" s="18">
-        <f t="shared" si="5"/>
-        <v>6</v>
+        <f t="shared" si="2"/>
+        <v>5.4</v>
       </c>
       <c r="E76" s="18">
-        <f t="shared" si="4"/>
-        <v>6</v>
+        <f t="shared" si="3"/>
+        <v>6.6000000000000005</v>
       </c>
       <c r="F76" s="19" t="s">
         <v>32</v>
@@ -3217,7 +3217,7 @@
       <c r="K76" s="13"/>
     </row>
     <row r="77" spans="1:11" ht="14.4" customHeight="1">
-      <c r="A77" s="68" t="s">
+      <c r="A77" s="57" t="s">
         <v>38</v>
       </c>
       <c r="B77" s="40" t="s">
@@ -3227,11 +3227,11 @@
         <v>0.25</v>
       </c>
       <c r="D77" s="41">
-        <f t="shared" ref="D77:D94" si="6">C77</f>
+        <f>C77</f>
         <v>0.25</v>
       </c>
       <c r="E77" s="41">
-        <f t="shared" si="2"/>
+        <f>C77</f>
         <v>0.25</v>
       </c>
       <c r="F77" s="42"/>
@@ -3240,7 +3240,7 @@
       </c>
     </row>
     <row r="78" spans="1:11">
-      <c r="A78" s="69"/>
+      <c r="A78" s="58"/>
       <c r="B78" s="40" t="s">
         <v>48</v>
       </c>
@@ -3248,11 +3248,11 @@
         <v>0.2</v>
       </c>
       <c r="D78" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="D78:D94" si="4">C78</f>
         <v>0.2</v>
       </c>
       <c r="E78" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="E78:E94" si="5">C78</f>
         <v>0.2</v>
       </c>
       <c r="F78" s="42"/>
@@ -3261,7 +3261,7 @@
       </c>
     </row>
     <row r="79" spans="1:11">
-      <c r="A79" s="69"/>
+      <c r="A79" s="58"/>
       <c r="B79" s="40" t="s">
         <v>40</v>
       </c>
@@ -3269,11 +3269,11 @@
         <v>0.2</v>
       </c>
       <c r="D79" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.2</v>
       </c>
       <c r="E79" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.2</v>
       </c>
       <c r="F79" s="42"/>
@@ -3282,7 +3282,7 @@
       </c>
     </row>
     <row r="80" spans="1:11">
-      <c r="A80" s="69"/>
+      <c r="A80" s="58"/>
       <c r="B80" s="40" t="s">
         <v>41</v>
       </c>
@@ -3290,11 +3290,11 @@
         <v>0.2</v>
       </c>
       <c r="D80" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.2</v>
       </c>
       <c r="E80" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.2</v>
       </c>
       <c r="F80" s="42"/>
@@ -3303,7 +3303,7 @@
       </c>
     </row>
     <row r="81" spans="1:11">
-      <c r="A81" s="69"/>
+      <c r="A81" s="58"/>
       <c r="B81" s="40" t="s">
         <v>42</v>
       </c>
@@ -3311,11 +3311,11 @@
         <v>0.5</v>
       </c>
       <c r="D81" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="E81" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="F81" s="42"/>
@@ -3324,7 +3324,7 @@
       </c>
     </row>
     <row r="82" spans="1:11">
-      <c r="A82" s="69"/>
+      <c r="A82" s="58"/>
       <c r="B82" s="40" t="s">
         <v>191</v>
       </c>
@@ -3332,11 +3332,11 @@
         <v>0.5</v>
       </c>
       <c r="D82" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="E82" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="F82" s="42"/>
@@ -3346,7 +3346,7 @@
       <c r="K82" s="13"/>
     </row>
     <row r="83" spans="1:11">
-      <c r="A83" s="69"/>
+      <c r="A83" s="58"/>
       <c r="B83" s="40" t="s">
         <v>43</v>
       </c>
@@ -3354,11 +3354,11 @@
         <v>0.25</v>
       </c>
       <c r="D83" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.25</v>
       </c>
       <c r="E83" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.25</v>
       </c>
       <c r="F83" s="42"/>
@@ -3368,7 +3368,7 @@
       <c r="K83" s="13"/>
     </row>
     <row r="84" spans="1:11">
-      <c r="A84" s="69"/>
+      <c r="A84" s="58"/>
       <c r="B84" s="40" t="s">
         <v>49</v>
       </c>
@@ -3376,11 +3376,11 @@
         <v>0.1</v>
       </c>
       <c r="D84" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
       <c r="E84" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
       <c r="F84" s="42"/>
@@ -3390,7 +3390,7 @@
       <c r="K84" s="13"/>
     </row>
     <row r="85" spans="1:11">
-      <c r="A85" s="69"/>
+      <c r="A85" s="58"/>
       <c r="B85" s="40" t="s">
         <v>44</v>
       </c>
@@ -3398,11 +3398,11 @@
         <v>0.1</v>
       </c>
       <c r="D85" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
       <c r="E85" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
       <c r="F85" s="42"/>
@@ -3412,7 +3412,7 @@
       <c r="K85" s="13"/>
     </row>
     <row r="86" spans="1:11">
-      <c r="A86" s="69"/>
+      <c r="A86" s="58"/>
       <c r="B86" s="40" t="s">
         <v>45</v>
       </c>
@@ -3420,11 +3420,11 @@
         <v>0.1</v>
       </c>
       <c r="D86" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
       <c r="E86" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
       <c r="F86" s="42"/>
@@ -3434,7 +3434,7 @@
       <c r="K86" s="13"/>
     </row>
     <row r="87" spans="1:11">
-      <c r="A87" s="69"/>
+      <c r="A87" s="58"/>
       <c r="B87" s="40" t="s">
         <v>46</v>
       </c>
@@ -3442,11 +3442,11 @@
         <v>0.45</v>
       </c>
       <c r="D87" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.45</v>
       </c>
       <c r="E87" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.45</v>
       </c>
       <c r="F87" s="42"/>
@@ -3455,7 +3455,7 @@
       </c>
     </row>
     <row r="88" spans="1:11">
-      <c r="A88" s="69"/>
+      <c r="A88" s="58"/>
       <c r="B88" s="40" t="s">
         <v>192</v>
       </c>
@@ -3463,11 +3463,11 @@
         <v>0.45</v>
       </c>
       <c r="D88" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.45</v>
       </c>
       <c r="E88" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.45</v>
       </c>
       <c r="F88" s="42"/>
@@ -3476,7 +3476,7 @@
       </c>
     </row>
     <row r="89" spans="1:11">
-      <c r="A89" s="69"/>
+      <c r="A89" s="58"/>
       <c r="B89" s="40" t="s">
         <v>47</v>
       </c>
@@ -3484,11 +3484,11 @@
         <v>0.5</v>
       </c>
       <c r="D89" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="E89" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="F89" s="42"/>
@@ -3497,7 +3497,7 @@
       </c>
     </row>
     <row r="90" spans="1:11">
-      <c r="A90" s="69"/>
+      <c r="A90" s="58"/>
       <c r="B90" s="40" t="s">
         <v>50</v>
       </c>
@@ -3505,11 +3505,11 @@
         <v>0.7</v>
       </c>
       <c r="D90" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
       <c r="E90" s="41">
-        <f t="shared" ref="E90:E94" si="7">C90</f>
+        <f t="shared" si="5"/>
         <v>0.7</v>
       </c>
       <c r="F90" s="42"/>
@@ -3518,7 +3518,7 @@
       </c>
     </row>
     <row r="91" spans="1:11">
-      <c r="A91" s="69"/>
+      <c r="A91" s="58"/>
       <c r="B91" s="40" t="s">
         <v>51</v>
       </c>
@@ -3526,11 +3526,11 @@
         <v>0.7</v>
       </c>
       <c r="D91" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
       <c r="E91" s="41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0.7</v>
       </c>
       <c r="F91" s="42"/>
@@ -3539,7 +3539,7 @@
       </c>
     </row>
     <row r="92" spans="1:11">
-      <c r="A92" s="69"/>
+      <c r="A92" s="58"/>
       <c r="B92" s="40" t="s">
         <v>52</v>
       </c>
@@ -3547,11 +3547,11 @@
         <v>0.7</v>
       </c>
       <c r="D92" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
       <c r="E92" s="41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0.7</v>
       </c>
       <c r="F92" s="42"/>
@@ -3560,7 +3560,7 @@
       </c>
     </row>
     <row r="93" spans="1:11">
-      <c r="A93" s="69"/>
+      <c r="A93" s="58"/>
       <c r="B93" s="40" t="s">
         <v>53</v>
       </c>
@@ -3568,11 +3568,11 @@
         <v>0.05</v>
       </c>
       <c r="D93" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.05</v>
       </c>
       <c r="E93" s="41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0.05</v>
       </c>
       <c r="F93" s="42"/>
@@ -3582,7 +3582,7 @@
       <c r="K93" s="13"/>
     </row>
     <row r="94" spans="1:11">
-      <c r="A94" s="69"/>
+      <c r="A94" s="58"/>
       <c r="B94" s="40" t="s">
         <v>193</v>
       </c>
@@ -3590,11 +3590,11 @@
         <v>0.05</v>
       </c>
       <c r="D94" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.05</v>
       </c>
       <c r="E94" s="41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0.05</v>
       </c>
       <c r="F94" s="42"/>
@@ -3649,16 +3649,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A22:A30"/>
+    <mergeCell ref="A31:A42"/>
+    <mergeCell ref="A43:A50"/>
     <mergeCell ref="J46:L46"/>
     <mergeCell ref="A57:A76"/>
     <mergeCell ref="A77:A94"/>
     <mergeCell ref="A51:A56"/>
     <mergeCell ref="A4:A18"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A22:A30"/>
-    <mergeCell ref="A31:A42"/>
-    <mergeCell ref="A43:A50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>